<commit_message>
edit mode fonctionne +/-, a corriger => index incrorect
</commit_message>
<xml_diff>
--- a/gantt-chart.xlsx
+++ b/gantt-chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20480" yWindow="5120" windowWidth="20480" windowHeight="20020" tabRatio="500"/>
+    <workbookView xWindow="3960" yWindow="700" windowWidth="20480" windowHeight="20020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="gantt" sheetId="1" r:id="rId1"/>
@@ -314,7 +314,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -405,6 +405,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="29">
     <border>
@@ -966,7 +972,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1238,61 +1244,70 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1807,7 +1822,7 @@
   <dimension ref="A1:EG67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.6640625" defaultRowHeight="41" customHeight="1" x14ac:dyDescent="0"/>
@@ -1877,210 +1892,210 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:137" s="1" customFormat="1" ht="29" customHeight="1">
-      <c r="A1" s="95" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="97" t="s">
+      <c r="A1" s="107" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="95" t="s">
+      <c r="C1" s="107" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="91">
+      <c r="D1" s="109">
         <v>42121</v>
       </c>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="91">
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="109"/>
+      <c r="J1" s="109"/>
+      <c r="K1" s="109">
         <f>D1+7</f>
         <v>42128</v>
       </c>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
-      <c r="N1" s="91"/>
-      <c r="O1" s="91"/>
-      <c r="P1" s="91"/>
-      <c r="Q1" s="91"/>
-      <c r="R1" s="91">
+      <c r="L1" s="109"/>
+      <c r="M1" s="109"/>
+      <c r="N1" s="109"/>
+      <c r="O1" s="109"/>
+      <c r="P1" s="109"/>
+      <c r="Q1" s="109"/>
+      <c r="R1" s="109">
         <f>K1+7</f>
         <v>42135</v>
       </c>
-      <c r="S1" s="91"/>
-      <c r="T1" s="91"/>
-      <c r="U1" s="91"/>
-      <c r="V1" s="91"/>
-      <c r="W1" s="91"/>
-      <c r="X1" s="91"/>
-      <c r="Y1" s="91">
+      <c r="S1" s="109"/>
+      <c r="T1" s="109"/>
+      <c r="U1" s="109"/>
+      <c r="V1" s="109"/>
+      <c r="W1" s="109"/>
+      <c r="X1" s="109"/>
+      <c r="Y1" s="109">
         <f t="shared" ref="Y1" si="0">R1+7</f>
         <v>42142</v>
       </c>
-      <c r="Z1" s="91"/>
-      <c r="AA1" s="91"/>
-      <c r="AB1" s="91"/>
-      <c r="AC1" s="91"/>
-      <c r="AD1" s="91"/>
-      <c r="AE1" s="91"/>
-      <c r="AF1" s="91">
+      <c r="Z1" s="109"/>
+      <c r="AA1" s="109"/>
+      <c r="AB1" s="109"/>
+      <c r="AC1" s="109"/>
+      <c r="AD1" s="109"/>
+      <c r="AE1" s="109"/>
+      <c r="AF1" s="109">
         <f t="shared" ref="AF1" si="1">Y1+7</f>
         <v>42149</v>
       </c>
-      <c r="AG1" s="91"/>
-      <c r="AH1" s="91"/>
-      <c r="AI1" s="91"/>
-      <c r="AJ1" s="91"/>
-      <c r="AK1" s="91"/>
-      <c r="AL1" s="91"/>
-      <c r="AM1" s="91">
+      <c r="AG1" s="109"/>
+      <c r="AH1" s="109"/>
+      <c r="AI1" s="109"/>
+      <c r="AJ1" s="109"/>
+      <c r="AK1" s="109"/>
+      <c r="AL1" s="109"/>
+      <c r="AM1" s="109">
         <f t="shared" ref="AM1" si="2">AF1+7</f>
         <v>42156</v>
       </c>
-      <c r="AN1" s="91"/>
-      <c r="AO1" s="91"/>
-      <c r="AP1" s="91"/>
-      <c r="AQ1" s="91"/>
-      <c r="AR1" s="91"/>
-      <c r="AS1" s="91"/>
-      <c r="AT1" s="91">
+      <c r="AN1" s="109"/>
+      <c r="AO1" s="109"/>
+      <c r="AP1" s="109"/>
+      <c r="AQ1" s="109"/>
+      <c r="AR1" s="109"/>
+      <c r="AS1" s="109"/>
+      <c r="AT1" s="109">
         <f t="shared" ref="AT1" si="3">AM1+7</f>
         <v>42163</v>
       </c>
-      <c r="AU1" s="91"/>
-      <c r="AV1" s="91"/>
-      <c r="AW1" s="91"/>
-      <c r="AX1" s="91"/>
-      <c r="AY1" s="91"/>
-      <c r="AZ1" s="91"/>
-      <c r="BA1" s="91">
+      <c r="AU1" s="109"/>
+      <c r="AV1" s="109"/>
+      <c r="AW1" s="109"/>
+      <c r="AX1" s="109"/>
+      <c r="AY1" s="109"/>
+      <c r="AZ1" s="109"/>
+      <c r="BA1" s="109">
         <f t="shared" ref="BA1" si="4">AT1+7</f>
         <v>42170</v>
       </c>
-      <c r="BB1" s="91"/>
-      <c r="BC1" s="91"/>
-      <c r="BD1" s="91"/>
-      <c r="BE1" s="91"/>
-      <c r="BF1" s="91"/>
-      <c r="BG1" s="91"/>
-      <c r="BH1" s="91">
+      <c r="BB1" s="109"/>
+      <c r="BC1" s="109"/>
+      <c r="BD1" s="109"/>
+      <c r="BE1" s="109"/>
+      <c r="BF1" s="109"/>
+      <c r="BG1" s="109"/>
+      <c r="BH1" s="109">
         <f t="shared" ref="BH1" si="5">BA1+7</f>
         <v>42177</v>
       </c>
-      <c r="BI1" s="91"/>
-      <c r="BJ1" s="91"/>
-      <c r="BK1" s="91"/>
-      <c r="BL1" s="91"/>
-      <c r="BM1" s="91"/>
-      <c r="BN1" s="91"/>
-      <c r="BO1" s="91">
+      <c r="BI1" s="109"/>
+      <c r="BJ1" s="109"/>
+      <c r="BK1" s="109"/>
+      <c r="BL1" s="109"/>
+      <c r="BM1" s="109"/>
+      <c r="BN1" s="109"/>
+      <c r="BO1" s="109">
         <f t="shared" ref="BO1" si="6">BH1+7</f>
         <v>42184</v>
       </c>
-      <c r="BP1" s="91"/>
-      <c r="BQ1" s="91"/>
-      <c r="BR1" s="91"/>
-      <c r="BS1" s="91"/>
-      <c r="BT1" s="91"/>
-      <c r="BU1" s="91"/>
-      <c r="BV1" s="91">
+      <c r="BP1" s="109"/>
+      <c r="BQ1" s="109"/>
+      <c r="BR1" s="109"/>
+      <c r="BS1" s="109"/>
+      <c r="BT1" s="109"/>
+      <c r="BU1" s="109"/>
+      <c r="BV1" s="109">
         <f t="shared" ref="BV1" si="7">BO1+7</f>
         <v>42191</v>
       </c>
-      <c r="BW1" s="91"/>
-      <c r="BX1" s="91"/>
-      <c r="BY1" s="91"/>
-      <c r="BZ1" s="91"/>
-      <c r="CA1" s="91"/>
-      <c r="CB1" s="91"/>
-      <c r="CC1" s="91">
+      <c r="BW1" s="109"/>
+      <c r="BX1" s="109"/>
+      <c r="BY1" s="109"/>
+      <c r="BZ1" s="109"/>
+      <c r="CA1" s="109"/>
+      <c r="CB1" s="109"/>
+      <c r="CC1" s="109">
         <f t="shared" ref="CC1" si="8">BV1+7</f>
         <v>42198</v>
       </c>
-      <c r="CD1" s="91"/>
-      <c r="CE1" s="91"/>
-      <c r="CF1" s="91"/>
-      <c r="CG1" s="91"/>
-      <c r="CH1" s="91"/>
-      <c r="CI1" s="91"/>
-      <c r="CJ1" s="91">
+      <c r="CD1" s="109"/>
+      <c r="CE1" s="109"/>
+      <c r="CF1" s="109"/>
+      <c r="CG1" s="109"/>
+      <c r="CH1" s="109"/>
+      <c r="CI1" s="109"/>
+      <c r="CJ1" s="109">
         <f t="shared" ref="CJ1" si="9">CC1+7</f>
         <v>42205</v>
       </c>
-      <c r="CK1" s="91"/>
-      <c r="CL1" s="91"/>
-      <c r="CM1" s="91"/>
-      <c r="CN1" s="91"/>
-      <c r="CO1" s="91"/>
-      <c r="CP1" s="91"/>
-      <c r="CQ1" s="91">
+      <c r="CK1" s="109"/>
+      <c r="CL1" s="109"/>
+      <c r="CM1" s="109"/>
+      <c r="CN1" s="109"/>
+      <c r="CO1" s="109"/>
+      <c r="CP1" s="109"/>
+      <c r="CQ1" s="109">
         <f t="shared" ref="CQ1" si="10">CJ1+7</f>
         <v>42212</v>
       </c>
-      <c r="CR1" s="91"/>
-      <c r="CS1" s="91"/>
-      <c r="CT1" s="91"/>
-      <c r="CU1" s="91"/>
-      <c r="CV1" s="91"/>
-      <c r="CW1" s="91"/>
-      <c r="CX1" s="91">
+      <c r="CR1" s="109"/>
+      <c r="CS1" s="109"/>
+      <c r="CT1" s="109"/>
+      <c r="CU1" s="109"/>
+      <c r="CV1" s="109"/>
+      <c r="CW1" s="109"/>
+      <c r="CX1" s="109">
         <f t="shared" ref="CX1" si="11">CQ1+7</f>
         <v>42219</v>
       </c>
-      <c r="CY1" s="91"/>
-      <c r="CZ1" s="91"/>
-      <c r="DA1" s="91"/>
-      <c r="DB1" s="91"/>
-      <c r="DC1" s="91"/>
-      <c r="DD1" s="91"/>
-      <c r="DE1" s="91">
+      <c r="CY1" s="109"/>
+      <c r="CZ1" s="109"/>
+      <c r="DA1" s="109"/>
+      <c r="DB1" s="109"/>
+      <c r="DC1" s="109"/>
+      <c r="DD1" s="109"/>
+      <c r="DE1" s="109">
         <f t="shared" ref="DE1" si="12">CX1+7</f>
         <v>42226</v>
       </c>
-      <c r="DF1" s="91"/>
-      <c r="DG1" s="91"/>
-      <c r="DH1" s="91"/>
-      <c r="DI1" s="91"/>
-      <c r="DJ1" s="91"/>
-      <c r="DK1" s="91"/>
-      <c r="DL1" s="91">
+      <c r="DF1" s="109"/>
+      <c r="DG1" s="109"/>
+      <c r="DH1" s="109"/>
+      <c r="DI1" s="109"/>
+      <c r="DJ1" s="109"/>
+      <c r="DK1" s="109"/>
+      <c r="DL1" s="109">
         <f t="shared" ref="DL1" si="13">DE1+7</f>
         <v>42233</v>
       </c>
-      <c r="DM1" s="91"/>
-      <c r="DN1" s="91"/>
-      <c r="DO1" s="91"/>
-      <c r="DP1" s="91"/>
-      <c r="DQ1" s="91"/>
-      <c r="DR1" s="91"/>
-      <c r="DS1" s="91">
+      <c r="DM1" s="109"/>
+      <c r="DN1" s="109"/>
+      <c r="DO1" s="109"/>
+      <c r="DP1" s="109"/>
+      <c r="DQ1" s="109"/>
+      <c r="DR1" s="109"/>
+      <c r="DS1" s="109">
         <f t="shared" ref="DS1" si="14">DL1+7</f>
         <v>42240</v>
       </c>
-      <c r="DT1" s="91"/>
-      <c r="DU1" s="91"/>
-      <c r="DV1" s="91"/>
-      <c r="DW1" s="91"/>
-      <c r="DX1" s="91"/>
-      <c r="DY1" s="91"/>
-      <c r="DZ1" s="91">
+      <c r="DT1" s="109"/>
+      <c r="DU1" s="109"/>
+      <c r="DV1" s="109"/>
+      <c r="DW1" s="109"/>
+      <c r="DX1" s="109"/>
+      <c r="DY1" s="109"/>
+      <c r="DZ1" s="109">
         <f t="shared" ref="DZ1" si="15">DS1+7</f>
         <v>42247</v>
       </c>
-      <c r="EA1" s="91"/>
-      <c r="EB1" s="91"/>
-      <c r="EC1" s="91"/>
-      <c r="ED1" s="91"/>
-      <c r="EE1" s="91"/>
-      <c r="EF1" s="91"/>
+      <c r="EA1" s="109"/>
+      <c r="EB1" s="109"/>
+      <c r="EC1" s="109"/>
+      <c r="ED1" s="109"/>
+      <c r="EE1" s="109"/>
+      <c r="EF1" s="109"/>
       <c r="EG1" s="27"/>
     </row>
     <row r="2" spans="1:137" s="9" customFormat="1" ht="34" customHeight="1" thickBot="1">
-      <c r="A2" s="96"/>
-      <c r="B2" s="98"/>
-      <c r="C2" s="96"/>
+      <c r="A2" s="108"/>
+      <c r="B2" s="106"/>
+      <c r="C2" s="108"/>
       <c r="D2" s="8" t="s">
         <v>1</v>
       </c>
@@ -2495,535 +2510,535 @@
         <v>26</v>
       </c>
       <c r="D3" s="20">
-        <f>SUM(D4:D56)</f>
+        <f t="shared" ref="D3:AI3" si="16">SUM(D4:D56)</f>
         <v>8</v>
       </c>
       <c r="E3" s="20">
-        <f>SUM(E4:E56)</f>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="F3" s="20">
-        <f>SUM(F4:F56)</f>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="G3" s="20">
-        <f>SUM(G4:G56)</f>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="H3" s="20">
-        <f>SUM(H4:H56)</f>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="I3" s="20">
-        <f>SUM(I4:I56)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="J3" s="20">
-        <f>SUM(J4:J56)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="K3" s="20">
-        <f>SUM(K4:K56)</f>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="L3" s="20">
-        <f>SUM(L4:L56)</f>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="M3" s="20">
-        <f>SUM(M4:M56)</f>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="N3" s="20">
-        <f>SUM(N4:N56)</f>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="O3" s="20">
-        <f>SUM(O4:O56)</f>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="P3" s="20">
-        <f>SUM(P4:P56)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="Q3" s="20">
-        <f>SUM(Q4:Q56)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="R3" s="20">
-        <f>SUM(R4:R56)</f>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="S3" s="20">
-        <f>SUM(S4:S56)</f>
+        <f t="shared" si="16"/>
         <v>4</v>
       </c>
       <c r="T3" s="20">
-        <f>SUM(T4:T56)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U3" s="20">
-        <f>SUM(U4:U56)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="V3" s="20">
-        <f>SUM(V4:V56)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="W3" s="20">
-        <f>SUM(W4:W56)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="X3" s="20">
-        <f>SUM(X4:X56)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="Y3" s="20">
-        <f>SUM(Y4:Y56)</f>
+        <f t="shared" si="16"/>
         <v>4</v>
       </c>
       <c r="Z3" s="20">
-        <f>SUM(Z4:Z56)</f>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="AA3" s="20">
-        <f>SUM(AA4:AA56)</f>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="AB3" s="20">
-        <f>SUM(AB4:AB56)</f>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="AC3" s="20">
-        <f>SUM(AC4:AC56)</f>
+        <f t="shared" si="16"/>
         <v>7</v>
       </c>
       <c r="AD3" s="20">
-        <f>SUM(AD4:AD56)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AE3" s="20">
-        <f>SUM(AE4:AE56)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AF3" s="20">
-        <f>SUM(AF4:AF56)</f>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="AG3" s="20">
-        <f>SUM(AG4:AG56)</f>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="AH3" s="20">
-        <f>SUM(AH4:AH56)</f>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="AI3" s="20">
-        <f>SUM(AI4:AI56)</f>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="AJ3" s="20">
-        <f>SUM(AJ4:AJ56)</f>
+        <f t="shared" ref="AJ3:BO3" si="17">SUM(AJ4:AJ56)</f>
         <v>8</v>
       </c>
       <c r="AK3" s="20">
-        <f>SUM(AK4:AK56)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AL3" s="20">
-        <f>SUM(AL4:AL56)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AM3" s="20">
-        <f>SUM(AM4:AM56)</f>
+        <f t="shared" si="17"/>
         <v>8</v>
       </c>
       <c r="AN3" s="20">
-        <f>SUM(AN4:AN56)</f>
+        <f t="shared" si="17"/>
         <v>8</v>
       </c>
       <c r="AO3" s="20">
-        <f>SUM(AO4:AO56)</f>
+        <f t="shared" si="17"/>
         <v>2</v>
       </c>
       <c r="AP3" s="20">
-        <f>SUM(AP4:AP56)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AQ3" s="20">
-        <f>SUM(AQ4:AQ56)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AR3" s="20">
-        <f>SUM(AR4:AR56)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AS3" s="20">
-        <f>SUM(AS4:AS56)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AT3" s="20">
-        <f>SUM(AT4:AT56)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AU3" s="20">
-        <f>SUM(AU4:AU56)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AV3" s="20">
-        <f>SUM(AV4:AV56)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AW3" s="20">
-        <f>SUM(AW4:AW56)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AX3" s="20">
-        <f>SUM(AX4:AX56)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AY3" s="20">
-        <f>SUM(AY4:AY56)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AZ3" s="20">
-        <f>SUM(AZ4:AZ56)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="BA3" s="20">
-        <f>SUM(BA4:BA56)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="BB3" s="20">
-        <f>SUM(BB4:BB56)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="BC3" s="20">
-        <f>SUM(BC4:BC56)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="BD3" s="20">
-        <f>SUM(BD4:BD56)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="BE3" s="20">
-        <f>SUM(BE4:BE56)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="BF3" s="20">
-        <f>SUM(BF4:BF56)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="BG3" s="20">
-        <f>SUM(BG4:BG56)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="BH3" s="20">
-        <f>SUM(BH4:BH56)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="BI3" s="20">
-        <f>SUM(BI4:BI56)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="BJ3" s="20">
-        <f>SUM(BJ4:BJ56)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="BK3" s="20">
-        <f>SUM(BK4:BK56)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="BL3" s="20">
-        <f>SUM(BL4:BL56)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="BM3" s="20">
-        <f>SUM(BM4:BM56)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="BN3" s="20">
-        <f>SUM(BN4:BN56)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="BO3" s="20">
-        <f>SUM(BO4:BO56)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="BP3" s="20">
-        <f>SUM(BP4:BP56)</f>
+        <f t="shared" ref="BP3:CU3" si="18">SUM(BP4:BP56)</f>
         <v>0</v>
       </c>
       <c r="BQ3" s="20">
-        <f>SUM(BQ4:BQ56)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="BR3" s="20">
-        <f>SUM(BR4:BR56)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="BS3" s="20">
-        <f>SUM(BS4:BS56)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="BT3" s="20">
-        <f>SUM(BT4:BT56)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="BU3" s="20">
-        <f>SUM(BU4:BU56)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="BV3" s="20">
-        <f>SUM(BV4:BV56)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="BW3" s="20">
-        <f>SUM(BW4:BW56)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="BX3" s="20">
-        <f>SUM(BX4:BX56)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="BY3" s="20">
-        <f>SUM(BY4:BY56)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="BZ3" s="20">
-        <f>SUM(BZ4:BZ56)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="CA3" s="20">
-        <f>SUM(CA4:CA56)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="CB3" s="20">
-        <f>SUM(CB4:CB56)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="CC3" s="20">
-        <f>SUM(CC4:CC56)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="CD3" s="20">
-        <f>SUM(CD4:CD56)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="CE3" s="20">
-        <f>SUM(CE4:CE56)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="CF3" s="20">
-        <f>SUM(CF4:CF56)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="CG3" s="20">
-        <f>SUM(CG4:CG56)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="CH3" s="20">
-        <f>SUM(CH4:CH56)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="CI3" s="20">
-        <f>SUM(CI4:CI56)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="CJ3" s="20">
-        <f>SUM(CJ4:CJ56)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="CK3" s="20">
-        <f>SUM(CK4:CK56)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="CL3" s="20">
-        <f>SUM(CL4:CL56)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="CM3" s="20">
-        <f>SUM(CM4:CM56)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="CN3" s="20">
-        <f>SUM(CN4:CN56)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="CO3" s="20">
-        <f>SUM(CO4:CO56)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="CP3" s="20">
-        <f>SUM(CP4:CP56)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="CQ3" s="20">
-        <f>SUM(CQ4:CQ56)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="CR3" s="20">
-        <f>SUM(CR4:CR56)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="CS3" s="20">
-        <f>SUM(CS4:CS56)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="CT3" s="20">
-        <f>SUM(CT4:CT56)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="CU3" s="20">
-        <f>SUM(CU4:CU56)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="CV3" s="20">
-        <f>SUM(CV4:CV56)</f>
+        <f t="shared" ref="CV3:EA3" si="19">SUM(CV4:CV56)</f>
         <v>0</v>
       </c>
       <c r="CW3" s="20">
-        <f>SUM(CW4:CW56)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="CX3" s="20">
-        <f>SUM(CX4:CX56)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="CY3" s="20">
-        <f>SUM(CY4:CY56)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="CZ3" s="20">
-        <f>SUM(CZ4:CZ56)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="DA3" s="20">
-        <f>SUM(DA4:DA56)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="DB3" s="20">
-        <f>SUM(DB4:DB56)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="DC3" s="20">
-        <f>SUM(DC4:DC56)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="DD3" s="20">
-        <f>SUM(DD4:DD56)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="DE3" s="20">
-        <f>SUM(DE4:DE56)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="DF3" s="20">
-        <f>SUM(DF4:DF56)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="DG3" s="20">
-        <f>SUM(DG4:DG56)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="DH3" s="20">
-        <f>SUM(DH4:DH56)</f>
+        <f t="shared" si="19"/>
         <v>8</v>
       </c>
       <c r="DI3" s="20">
-        <f>SUM(DI4:DI56)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="DJ3" s="20">
-        <f>SUM(DJ4:DJ56)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="DK3" s="20">
-        <f>SUM(DK4:DK56)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="DL3" s="20">
-        <f>SUM(DL4:DL56)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="DM3" s="20">
-        <f>SUM(DM4:DM56)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="DN3" s="20">
-        <f>SUM(DN4:DN56)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="DO3" s="20">
-        <f>SUM(DO4:DO56)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="DP3" s="20">
-        <f>SUM(DP4:DP56)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="DQ3" s="20">
-        <f>SUM(DQ4:DQ56)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="DR3" s="20">
-        <f>SUM(DR4:DR56)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="DS3" s="20">
-        <f>SUM(DS4:DS56)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="DT3" s="20">
-        <f>SUM(DT4:DT56)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="DU3" s="20">
-        <f>SUM(DU4:DU56)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="DV3" s="20">
-        <f>SUM(DV4:DV56)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="DW3" s="20">
-        <f>SUM(DW4:DW56)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="DX3" s="20">
-        <f>SUM(DX4:DX56)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="DY3" s="20">
-        <f>SUM(DY4:DY56)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="DZ3" s="20">
-        <f>SUM(DZ4:DZ56)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="EA3" s="20">
-        <f>SUM(EA4:EA56)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="EB3" s="20">
-        <f>SUM(EB4:EB56)</f>
+        <f t="shared" ref="EB3:FG3" si="20">SUM(EB4:EB56)</f>
         <v>0</v>
       </c>
       <c r="EC3" s="20">
-        <f>SUM(EC4:EC56)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="ED3" s="20">
-        <f>SUM(ED4:ED56)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="EE3" s="20">
-        <f>SUM(EE4:EE56)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="EF3" s="20">
-        <f>SUM(EF4:EF56)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="EG3" s="20"/>
@@ -3039,10 +3054,10 @@
         <f>SUM(D4:EF4)</f>
         <v>8</v>
       </c>
-      <c r="D4" s="105">
+      <c r="D4" s="97">
         <v>8</v>
       </c>
-      <c r="E4" s="106"/>
+      <c r="E4" s="98"/>
       <c r="F4" s="77"/>
       <c r="J4" s="30"/>
       <c r="K4" s="17"/>
@@ -3095,11 +3110,11 @@
         <v>2</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="107">
+      <c r="E5" s="99">
         <v>2</v>
       </c>
-      <c r="F5" s="106"/>
-      <c r="G5" s="107"/>
+      <c r="F5" s="98"/>
+      <c r="G5" s="99"/>
     </row>
     <row r="6" spans="1:137" s="13" customFormat="1" ht="41" customHeight="1" thickBot="1">
       <c r="A6" s="10" t="s">
@@ -3112,17 +3127,17 @@
         <f>SUM(D6:EF6)</f>
         <v>16</v>
       </c>
-      <c r="D6" s="108"/>
-      <c r="E6" s="108">
+      <c r="D6" s="100"/>
+      <c r="E6" s="100">
         <v>6</v>
       </c>
-      <c r="F6" s="109">
+      <c r="F6" s="101">
         <v>8</v>
       </c>
-      <c r="G6" s="108">
+      <c r="G6" s="100">
         <v>2</v>
       </c>
-      <c r="I6" s="64"/>
+      <c r="I6" s="99"/>
       <c r="J6" s="70"/>
       <c r="K6" s="71"/>
       <c r="Q6" s="32"/>
@@ -3226,11 +3241,12 @@
         <v>4</v>
       </c>
       <c r="D8" s="17"/>
-      <c r="G8" s="25">
+      <c r="G8" s="110">
         <v>4</v>
       </c>
+      <c r="H8" s="110"/>
       <c r="J8" s="30"/>
-      <c r="K8" s="17"/>
+      <c r="K8" s="112"/>
       <c r="L8" s="22"/>
       <c r="N8" s="37"/>
       <c r="O8" s="37"/>
@@ -3295,13 +3311,13 @@
         <f>SUM(D9:EF9)</f>
         <v>12</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="99">
         <v>2</v>
       </c>
-      <c r="H9" s="23">
+      <c r="H9" s="99">
         <v>8</v>
       </c>
-      <c r="K9" s="33">
+      <c r="K9" s="111">
         <v>2</v>
       </c>
       <c r="N9" s="64"/>
@@ -3337,7 +3353,7 @@
       </c>
       <c r="D10" s="12"/>
       <c r="J10" s="32"/>
-      <c r="K10" s="26">
+      <c r="K10" s="101">
         <v>6</v>
       </c>
       <c r="L10" s="24">
@@ -3455,7 +3471,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="15">
-        <f t="shared" ref="C12:C16" si="16">SUM(D12:EF12)</f>
+        <f t="shared" ref="C12:C16" si="21">SUM(D12:EF12)</f>
         <v>4</v>
       </c>
       <c r="D12" s="17"/>
@@ -3517,7 +3533,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>8</v>
       </c>
       <c r="G13" s="35"/>
@@ -3548,7 +3564,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>8</v>
       </c>
       <c r="G14" s="35"/>
@@ -3559,7 +3575,7 @@
       <c r="L14" s="35"/>
       <c r="M14" s="35"/>
       <c r="N14" s="35"/>
-      <c r="O14" s="99">
+      <c r="O14" s="91">
         <v>8</v>
       </c>
       <c r="P14" s="35"/>
@@ -3577,7 +3593,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>6</v>
       </c>
       <c r="G15" s="35"/>
@@ -3606,7 +3622,7 @@
         <v>5</v>
       </c>
       <c r="C16" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>4</v>
       </c>
       <c r="D16" s="12"/>
@@ -3722,7 +3738,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="15">
-        <f t="shared" ref="C18:C19" si="17">SUM(D18:EF18)</f>
+        <f t="shared" ref="C18:C19" si="22">SUM(D18:EF18)</f>
         <v>4</v>
       </c>
       <c r="D18" s="4"/>
@@ -3734,13 +3750,13 @@
       <c r="J18" s="36"/>
       <c r="K18" s="4"/>
       <c r="L18" s="35"/>
-      <c r="T18" s="92" t="s">
+      <c r="T18" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="U18" s="93"/>
-      <c r="V18" s="93"/>
-      <c r="W18" s="93"/>
-      <c r="X18" s="94"/>
+      <c r="U18" s="103"/>
+      <c r="V18" s="103"/>
+      <c r="W18" s="103"/>
+      <c r="X18" s="104"/>
       <c r="Y18" s="33">
         <v>4</v>
       </c>
@@ -3754,7 +3770,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>12</v>
       </c>
       <c r="D19" s="73"/>
@@ -3768,13 +3784,13 @@
       <c r="L19" s="34"/>
       <c r="Q19" s="32"/>
       <c r="R19" s="12"/>
-      <c r="T19" s="92" t="s">
+      <c r="T19" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="U19" s="93"/>
-      <c r="V19" s="93"/>
-      <c r="W19" s="93"/>
-      <c r="X19" s="94"/>
+      <c r="U19" s="103"/>
+      <c r="V19" s="103"/>
+      <c r="W19" s="103"/>
+      <c r="X19" s="104"/>
       <c r="Y19" s="12"/>
       <c r="Z19" s="24">
         <v>8</v>
@@ -3876,7 +3892,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="15">
-        <f t="shared" ref="C21:C40" si="18">SUM(D21:EF21)</f>
+        <f t="shared" ref="C21:C40" si="23">SUM(D21:EF21)</f>
         <v>2</v>
       </c>
       <c r="D21" s="17"/>
@@ -3895,7 +3911,7 @@
       <c r="AA21" s="38">
         <v>2</v>
       </c>
-      <c r="AB21" s="100"/>
+      <c r="AB21" s="92"/>
       <c r="AE21" s="74"/>
       <c r="AF21" s="75"/>
       <c r="AG21" s="77"/>
@@ -3941,7 +3957,7 @@
         <v>4</v>
       </c>
       <c r="C22" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="S22" s="35"/>
@@ -3955,7 +3971,7 @@
       <c r="AA22" s="33">
         <v>1</v>
       </c>
-      <c r="AB22" s="101"/>
+      <c r="AB22" s="93"/>
       <c r="AE22" s="36"/>
       <c r="AF22" s="4"/>
       <c r="AG22" s="77"/>
@@ -3971,7 +3987,7 @@
         <v>5</v>
       </c>
       <c r="C23" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>6</v>
       </c>
       <c r="S23" s="35"/>
@@ -3989,7 +4005,7 @@
         <v>5</v>
       </c>
       <c r="AE23" s="36"/>
-      <c r="AF23" s="102"/>
+      <c r="AF23" s="94"/>
       <c r="AG23" s="35"/>
       <c r="AH23" s="77"/>
       <c r="AI23" s="35"/>
@@ -4003,7 +4019,7 @@
         <v>4</v>
       </c>
       <c r="C24" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="S24" s="35"/>
@@ -4034,7 +4050,7 @@
         <v>4</v>
       </c>
       <c r="C25" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="D25" s="12"/>
@@ -4058,7 +4074,7 @@
         <v>1</v>
       </c>
       <c r="AE25" s="72"/>
-      <c r="AF25" s="103"/>
+      <c r="AF25" s="95"/>
       <c r="AG25" s="34"/>
       <c r="AH25" s="77"/>
       <c r="AI25" s="34"/>
@@ -4154,7 +4170,7 @@
         <v>4</v>
       </c>
       <c r="C27" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="D27" s="17"/>
@@ -4169,7 +4185,7 @@
       </c>
       <c r="AD27" s="37"/>
       <c r="AE27" s="74"/>
-      <c r="AF27" s="104"/>
+      <c r="AF27" s="96"/>
       <c r="AG27" s="37"/>
       <c r="AH27" s="77"/>
       <c r="AI27" s="37"/>
@@ -4214,7 +4230,7 @@
         <v>3</v>
       </c>
       <c r="C28" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>4</v>
       </c>
       <c r="AC28" s="23">
@@ -4222,7 +4238,7 @@
       </c>
       <c r="AD28" s="35"/>
       <c r="AE28" s="36"/>
-      <c r="AF28" s="102"/>
+      <c r="AF28" s="94"/>
       <c r="AG28" s="37"/>
       <c r="AH28" s="35"/>
       <c r="AI28" s="77"/>
@@ -4237,7 +4253,7 @@
         <v>5</v>
       </c>
       <c r="C29" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>4</v>
       </c>
       <c r="D29" s="12"/>
@@ -4349,7 +4365,7 @@
         <v>4</v>
       </c>
       <c r="C31" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="D31" s="17"/>
@@ -4408,7 +4424,7 @@
         <v>3</v>
       </c>
       <c r="C32" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>4</v>
       </c>
       <c r="AF32" s="33">
@@ -4433,7 +4449,7 @@
         <v>5</v>
       </c>
       <c r="C33" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>4</v>
       </c>
       <c r="D33" s="12"/>
@@ -4544,7 +4560,7 @@
         <v>4</v>
       </c>
       <c r="C35" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>4</v>
       </c>
       <c r="D35" s="17"/>
@@ -4607,7 +4623,7 @@
         <v>3</v>
       </c>
       <c r="C36" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>4</v>
       </c>
       <c r="AH36" s="23">
@@ -4630,7 +4646,7 @@
         <v>5</v>
       </c>
       <c r="C37" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>4</v>
       </c>
       <c r="D37" s="12"/>
@@ -4651,7 +4667,7 @@
       <c r="AJ37" s="37"/>
       <c r="AK37" s="34"/>
       <c r="AL37" s="72"/>
-      <c r="AM37" s="103"/>
+      <c r="AM37" s="95"/>
       <c r="AN37" s="34"/>
       <c r="AO37" s="77"/>
       <c r="AP37" s="34"/>
@@ -4744,7 +4760,7 @@
         <v>8</v>
       </c>
       <c r="C39" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>8</v>
       </c>
       <c r="D39" s="17"/>
@@ -4806,7 +4822,7 @@
         <v>3</v>
       </c>
       <c r="C40" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>4</v>
       </c>
       <c r="D40" s="12"/>
@@ -4824,7 +4840,7 @@
       </c>
       <c r="AK40" s="34"/>
       <c r="AL40" s="72"/>
-      <c r="AM40" s="103"/>
+      <c r="AM40" s="95"/>
       <c r="AN40" s="37"/>
       <c r="AO40" s="77"/>
       <c r="AP40" s="34"/>
@@ -6351,14 +6367,12 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="T19:X19"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:J1"/>
-    <mergeCell ref="K1:Q1"/>
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="T18:X18"/>
+    <mergeCell ref="DE1:DK1"/>
+    <mergeCell ref="DL1:DR1"/>
+    <mergeCell ref="DS1:DY1"/>
+    <mergeCell ref="DZ1:EF1"/>
+    <mergeCell ref="CQ1:CW1"/>
+    <mergeCell ref="CX1:DD1"/>
     <mergeCell ref="BO1:BU1"/>
     <mergeCell ref="BV1:CB1"/>
     <mergeCell ref="CC1:CI1"/>
@@ -6369,12 +6383,14 @@
     <mergeCell ref="AT1:AZ1"/>
     <mergeCell ref="BA1:BG1"/>
     <mergeCell ref="BH1:BN1"/>
-    <mergeCell ref="DE1:DK1"/>
-    <mergeCell ref="DL1:DR1"/>
-    <mergeCell ref="DS1:DY1"/>
-    <mergeCell ref="DZ1:EF1"/>
-    <mergeCell ref="CQ1:CW1"/>
-    <mergeCell ref="CX1:DD1"/>
+    <mergeCell ref="T19:X19"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="K1:Q1"/>
+    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="T18:X18"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
finitions vue interventions, détection problème suppresion quand plusieurs interventions, problème reste à régler.
</commit_message>
<xml_diff>
--- a/gantt-chart.xlsx
+++ b/gantt-chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="700" windowWidth="20480" windowHeight="20020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="gantt" sheetId="1" r:id="rId1"/>
@@ -124,9 +124,6 @@
     <t>3.4 Enregistrement des données entrées</t>
   </si>
   <si>
-    <t>3.5Modification des mesures/données</t>
-  </si>
-  <si>
     <t>5 Réserves | 4.5-4.6</t>
   </si>
   <si>
@@ -245,6 +242,9 @@
   </si>
   <si>
     <t>9.2 Gestion des données transitoires pour assurer la navigation</t>
+  </si>
+  <si>
+    <t>3.5 Modification des mesures/données</t>
   </si>
 </sst>
 </file>
@@ -1821,8 +1821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EG67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.6640625" defaultRowHeight="41" customHeight="1" x14ac:dyDescent="0"/>
@@ -3356,7 +3356,7 @@
       <c r="K10" s="101">
         <v>6</v>
       </c>
-      <c r="L10" s="24">
+      <c r="L10" s="100">
         <v>6</v>
       </c>
       <c r="N10" s="34"/>
@@ -3616,7 +3616,7 @@
     </row>
     <row r="16" spans="1:137" s="13" customFormat="1" ht="41" customHeight="1" thickBot="1">
       <c r="A16" s="10" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="B16" s="68">
         <v>5</v>
@@ -3680,7 +3680,7 @@
     </row>
     <row r="17" spans="1:137" s="21" customFormat="1" ht="41" customHeight="1" thickBot="1">
       <c r="A17" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" s="19">
         <f>SUM(B18:B19)</f>
@@ -3732,7 +3732,7 @@
     </row>
     <row r="18" spans="1:137" ht="41" customHeight="1">
       <c r="A18" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="15">
         <v>2</v>
@@ -3764,7 +3764,7 @@
     </row>
     <row r="19" spans="1:137" s="13" customFormat="1" ht="41" customHeight="1" thickBot="1">
       <c r="A19" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="68">
         <v>2</v>
@@ -3834,7 +3834,7 @@
     </row>
     <row r="20" spans="1:137" s="21" customFormat="1" ht="41" customHeight="1" thickBot="1">
       <c r="A20" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" s="19">
         <f>SUM(B21:B23)</f>
@@ -3886,7 +3886,7 @@
     </row>
     <row r="21" spans="1:137" s="16" customFormat="1" ht="41" customHeight="1">
       <c r="A21" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" s="15">
         <v>4</v>
@@ -3951,7 +3951,7 @@
     </row>
     <row r="22" spans="1:137" ht="41" customHeight="1">
       <c r="A22" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" s="15">
         <v>4</v>
@@ -3981,7 +3981,7 @@
     </row>
     <row r="23" spans="1:137" ht="41" customHeight="1">
       <c r="A23" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" s="15">
         <v>5</v>
@@ -4013,7 +4013,7 @@
     </row>
     <row r="24" spans="1:137" ht="41" customHeight="1">
       <c r="A24" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24" s="15">
         <v>4</v>
@@ -4044,7 +4044,7 @@
     </row>
     <row r="25" spans="1:137" s="13" customFormat="1" ht="41" customHeight="1" thickBot="1">
       <c r="A25" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" s="68">
         <v>4</v>
@@ -4112,7 +4112,7 @@
     </row>
     <row r="26" spans="1:137" s="21" customFormat="1" ht="41" customHeight="1" thickBot="1">
       <c r="A26" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="19">
         <f>SUM(B27:B29)</f>
@@ -4164,7 +4164,7 @@
     </row>
     <row r="27" spans="1:137" s="16" customFormat="1" ht="41" customHeight="1">
       <c r="A27" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B27" s="15">
         <v>4</v>
@@ -4224,7 +4224,7 @@
     </row>
     <row r="28" spans="1:137" ht="41" customHeight="1">
       <c r="A28" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28" s="15">
         <v>3</v>
@@ -4247,7 +4247,7 @@
     </row>
     <row r="29" spans="1:137" s="13" customFormat="1" ht="41" customHeight="1" thickBot="1">
       <c r="A29" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B29" s="68">
         <v>5</v>
@@ -4307,7 +4307,7 @@
     </row>
     <row r="30" spans="1:137" s="21" customFormat="1" ht="41" customHeight="1" thickBot="1">
       <c r="A30" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B30" s="19">
         <f>SUM(B31:B33)</f>
@@ -4359,7 +4359,7 @@
     </row>
     <row r="31" spans="1:137" s="16" customFormat="1" ht="41" customHeight="1">
       <c r="A31" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B31" s="15">
         <v>4</v>
@@ -4418,7 +4418,7 @@
     </row>
     <row r="32" spans="1:137" ht="41" customHeight="1">
       <c r="A32" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B32" s="15">
         <v>3</v>
@@ -4443,7 +4443,7 @@
     </row>
     <row r="33" spans="1:137" s="13" customFormat="1" ht="41" customHeight="1" thickBot="1">
       <c r="A33" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B33" s="68">
         <v>5</v>
@@ -4502,7 +4502,7 @@
     </row>
     <row r="34" spans="1:137" s="21" customFormat="1" ht="41" customHeight="1" thickBot="1">
       <c r="A34" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B34" s="19">
         <f>SUM(B35:B37)</f>
@@ -4554,7 +4554,7 @@
     </row>
     <row r="35" spans="1:137" s="16" customFormat="1" ht="41" customHeight="1">
       <c r="A35" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B35" s="15">
         <v>4</v>
@@ -4617,7 +4617,7 @@
     </row>
     <row r="36" spans="1:137" ht="41" customHeight="1">
       <c r="A36" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B36" s="15">
         <v>3</v>
@@ -4640,7 +4640,7 @@
     </row>
     <row r="37" spans="1:137" s="13" customFormat="1" ht="41" customHeight="1" thickBot="1">
       <c r="A37" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B37" s="68">
         <v>5</v>
@@ -4702,7 +4702,7 @@
     </row>
     <row r="38" spans="1:137" s="21" customFormat="1" ht="41" customHeight="1" thickBot="1">
       <c r="A38" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B38" s="19">
         <f>SUM(B39:B40)</f>
@@ -4754,7 +4754,7 @@
     </row>
     <row r="39" spans="1:137" s="16" customFormat="1" ht="41" customHeight="1">
       <c r="A39" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B39" s="15">
         <v>8</v>
@@ -4816,7 +4816,7 @@
     </row>
     <row r="40" spans="1:137" s="13" customFormat="1" ht="41" customHeight="1" thickBot="1">
       <c r="A40" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B40" s="68">
         <v>3</v>
@@ -4876,7 +4876,7 @@
     </row>
     <row r="41" spans="1:137" s="21" customFormat="1" ht="41" customHeight="1" thickBot="1">
       <c r="A41" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B41" s="19">
         <f>SUM(B42:B44)</f>
@@ -4928,7 +4928,7 @@
     </row>
     <row r="42" spans="1:137" s="16" customFormat="1" ht="41" customHeight="1">
       <c r="A42" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B42" s="15">
         <v>4</v>
@@ -4990,7 +4990,7 @@
     </row>
     <row r="43" spans="1:137" ht="41" customHeight="1">
       <c r="A43" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B43" s="15">
         <v>6</v>
@@ -5014,7 +5014,7 @@
     </row>
     <row r="44" spans="1:137" s="13" customFormat="1" ht="41" customHeight="1" thickBot="1">
       <c r="A44" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B44" s="68">
         <v>6</v>
@@ -5076,7 +5076,7 @@
     </row>
     <row r="45" spans="1:137" s="21" customFormat="1" ht="41" customHeight="1" thickBot="1">
       <c r="A45" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B45" s="19">
         <f>SUM(B46:B48)</f>
@@ -5128,7 +5128,7 @@
     </row>
     <row r="46" spans="1:137" s="16" customFormat="1" ht="41" customHeight="1">
       <c r="A46" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B46" s="15">
         <v>7</v>
@@ -5267,7 +5267,7 @@
     </row>
     <row r="47" spans="1:137" ht="41" customHeight="1">
       <c r="A47" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B47" s="5">
         <v>7</v>
@@ -5402,7 +5402,7 @@
     </row>
     <row r="48" spans="1:137" s="13" customFormat="1" ht="41" customHeight="1" thickBot="1">
       <c r="A48" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B48" s="11">
         <v>10</v>
@@ -5541,7 +5541,7 @@
     </row>
     <row r="49" spans="1:137" s="21" customFormat="1" ht="41" customHeight="1" thickBot="1">
       <c r="A49" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B49" s="19">
         <f>SUM(B50:B53)</f>
@@ -5593,7 +5593,7 @@
     </row>
     <row r="50" spans="1:137" s="16" customFormat="1" ht="41" customHeight="1">
       <c r="A50" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B50" s="15">
         <v>1</v>
@@ -5693,7 +5693,7 @@
     </row>
     <row r="51" spans="1:137" ht="41" customHeight="1">
       <c r="A51" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B51" s="5">
         <v>5</v>
@@ -5774,7 +5774,7 @@
     </row>
     <row r="52" spans="1:137" ht="41" customHeight="1">
       <c r="A52" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B52" s="5">
         <v>9</v>
@@ -5855,7 +5855,7 @@
     </row>
     <row r="53" spans="1:137" s="13" customFormat="1" ht="41" customHeight="1" thickBot="1">
       <c r="A53" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B53" s="11">
         <v>7</v>
@@ -5955,7 +5955,7 @@
     </row>
     <row r="54" spans="1:137" s="21" customFormat="1" ht="41" customHeight="1" thickBot="1">
       <c r="A54" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B54" s="19">
         <f>SUM(B55:B56)</f>
@@ -6007,7 +6007,7 @@
     </row>
     <row r="55" spans="1:137" s="16" customFormat="1" ht="41" customHeight="1">
       <c r="A55" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B55" s="15">
         <v>1</v>
@@ -6071,7 +6071,7 @@
     </row>
     <row r="56" spans="1:137" s="13" customFormat="1" ht="41" customHeight="1" thickBot="1">
       <c r="A56" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B56" s="11">
         <v>6</v>

</xml_diff>

<commit_message>
ajout fonction notes, suppression et sauvegarde dans array tampon des act terminés
</commit_message>
<xml_diff>
--- a/gantt-chart.xlsx
+++ b/gantt-chart.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="75">
   <si>
     <t>Nom de la tache</t>
   </si>
@@ -245,6 +245,9 @@
   </si>
   <si>
     <t>3.5 Modification des mesures/données</t>
+  </si>
+  <si>
+    <t>En cours après deadline</t>
   </si>
 </sst>
 </file>
@@ -314,7 +317,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -405,6 +408,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="29">
     <border>
@@ -785,7 +794,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="179">
+  <cellStyleXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -965,8 +974,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1277,6 +1288,9 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1298,11 +1312,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="179">
+  <cellStyles count="181">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -1392,6 +1412,7 @@
     <cellStyle name="Lien hypertexte" xfId="173" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="179" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -1481,6 +1502,7 @@
     <cellStyle name="Lien hypertexte visité" xfId="174" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="176" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="180" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1813,8 +1835,8 @@
   <dimension ref="A1:EG67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O11" sqref="O11"/>
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.6640625" defaultRowHeight="41" customHeight="1" x14ac:dyDescent="0"/>
@@ -1884,210 +1906,210 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:137" s="1" customFormat="1" ht="29" customHeight="1">
-      <c r="A1" s="109" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="107" t="s">
+      <c r="A1" s="110" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="108" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="109" t="s">
+      <c r="C1" s="110" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="111">
+      <c r="D1" s="104">
         <v>42121</v>
       </c>
-      <c r="E1" s="111"/>
-      <c r="F1" s="111"/>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
-      <c r="I1" s="111"/>
-      <c r="J1" s="111"/>
-      <c r="K1" s="111">
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="104">
         <f>D1+7</f>
         <v>42128</v>
       </c>
-      <c r="L1" s="111"/>
-      <c r="M1" s="111"/>
-      <c r="N1" s="111"/>
-      <c r="O1" s="111"/>
-      <c r="P1" s="111"/>
-      <c r="Q1" s="111"/>
-      <c r="R1" s="111">
+      <c r="L1" s="104"/>
+      <c r="M1" s="104"/>
+      <c r="N1" s="104"/>
+      <c r="O1" s="104"/>
+      <c r="P1" s="104"/>
+      <c r="Q1" s="104"/>
+      <c r="R1" s="104">
         <f>K1+7</f>
         <v>42135</v>
       </c>
-      <c r="S1" s="111"/>
-      <c r="T1" s="111"/>
-      <c r="U1" s="111"/>
-      <c r="V1" s="111"/>
-      <c r="W1" s="111"/>
-      <c r="X1" s="111"/>
-      <c r="Y1" s="111">
+      <c r="S1" s="104"/>
+      <c r="T1" s="104"/>
+      <c r="U1" s="104"/>
+      <c r="V1" s="104"/>
+      <c r="W1" s="104"/>
+      <c r="X1" s="104"/>
+      <c r="Y1" s="104">
         <f t="shared" ref="Y1" si="0">R1+7</f>
         <v>42142</v>
       </c>
-      <c r="Z1" s="111"/>
-      <c r="AA1" s="111"/>
-      <c r="AB1" s="111"/>
-      <c r="AC1" s="111"/>
-      <c r="AD1" s="111"/>
-      <c r="AE1" s="111"/>
-      <c r="AF1" s="111">
+      <c r="Z1" s="104"/>
+      <c r="AA1" s="104"/>
+      <c r="AB1" s="104"/>
+      <c r="AC1" s="104"/>
+      <c r="AD1" s="104"/>
+      <c r="AE1" s="104"/>
+      <c r="AF1" s="104">
         <f t="shared" ref="AF1" si="1">Y1+7</f>
         <v>42149</v>
       </c>
-      <c r="AG1" s="111"/>
-      <c r="AH1" s="111"/>
-      <c r="AI1" s="111"/>
-      <c r="AJ1" s="111"/>
-      <c r="AK1" s="111"/>
-      <c r="AL1" s="111"/>
-      <c r="AM1" s="111">
+      <c r="AG1" s="104"/>
+      <c r="AH1" s="104"/>
+      <c r="AI1" s="104"/>
+      <c r="AJ1" s="104"/>
+      <c r="AK1" s="104"/>
+      <c r="AL1" s="104"/>
+      <c r="AM1" s="104">
         <f t="shared" ref="AM1" si="2">AF1+7</f>
         <v>42156</v>
       </c>
-      <c r="AN1" s="111"/>
-      <c r="AO1" s="111"/>
-      <c r="AP1" s="111"/>
-      <c r="AQ1" s="111"/>
-      <c r="AR1" s="111"/>
-      <c r="AS1" s="111"/>
-      <c r="AT1" s="111">
+      <c r="AN1" s="104"/>
+      <c r="AO1" s="104"/>
+      <c r="AP1" s="104"/>
+      <c r="AQ1" s="104"/>
+      <c r="AR1" s="104"/>
+      <c r="AS1" s="104"/>
+      <c r="AT1" s="104">
         <f t="shared" ref="AT1" si="3">AM1+7</f>
         <v>42163</v>
       </c>
-      <c r="AU1" s="111"/>
-      <c r="AV1" s="111"/>
-      <c r="AW1" s="111"/>
-      <c r="AX1" s="111"/>
-      <c r="AY1" s="111"/>
-      <c r="AZ1" s="111"/>
-      <c r="BA1" s="111">
+      <c r="AU1" s="104"/>
+      <c r="AV1" s="104"/>
+      <c r="AW1" s="104"/>
+      <c r="AX1" s="104"/>
+      <c r="AY1" s="104"/>
+      <c r="AZ1" s="104"/>
+      <c r="BA1" s="104">
         <f t="shared" ref="BA1" si="4">AT1+7</f>
         <v>42170</v>
       </c>
-      <c r="BB1" s="111"/>
-      <c r="BC1" s="111"/>
-      <c r="BD1" s="111"/>
-      <c r="BE1" s="111"/>
-      <c r="BF1" s="111"/>
-      <c r="BG1" s="111"/>
-      <c r="BH1" s="111">
+      <c r="BB1" s="104"/>
+      <c r="BC1" s="104"/>
+      <c r="BD1" s="104"/>
+      <c r="BE1" s="104"/>
+      <c r="BF1" s="104"/>
+      <c r="BG1" s="104"/>
+      <c r="BH1" s="104">
         <f t="shared" ref="BH1" si="5">BA1+7</f>
         <v>42177</v>
       </c>
-      <c r="BI1" s="111"/>
-      <c r="BJ1" s="111"/>
-      <c r="BK1" s="111"/>
-      <c r="BL1" s="111"/>
-      <c r="BM1" s="111"/>
-      <c r="BN1" s="111"/>
-      <c r="BO1" s="111">
+      <c r="BI1" s="104"/>
+      <c r="BJ1" s="104"/>
+      <c r="BK1" s="104"/>
+      <c r="BL1" s="104"/>
+      <c r="BM1" s="104"/>
+      <c r="BN1" s="104"/>
+      <c r="BO1" s="104">
         <f t="shared" ref="BO1" si="6">BH1+7</f>
         <v>42184</v>
       </c>
-      <c r="BP1" s="111"/>
-      <c r="BQ1" s="111"/>
-      <c r="BR1" s="111"/>
-      <c r="BS1" s="111"/>
-      <c r="BT1" s="111"/>
-      <c r="BU1" s="111"/>
-      <c r="BV1" s="111">
+      <c r="BP1" s="104"/>
+      <c r="BQ1" s="104"/>
+      <c r="BR1" s="104"/>
+      <c r="BS1" s="104"/>
+      <c r="BT1" s="104"/>
+      <c r="BU1" s="104"/>
+      <c r="BV1" s="104">
         <f t="shared" ref="BV1" si="7">BO1+7</f>
         <v>42191</v>
       </c>
-      <c r="BW1" s="111"/>
-      <c r="BX1" s="111"/>
-      <c r="BY1" s="111"/>
-      <c r="BZ1" s="111"/>
-      <c r="CA1" s="111"/>
-      <c r="CB1" s="111"/>
-      <c r="CC1" s="111">
+      <c r="BW1" s="104"/>
+      <c r="BX1" s="104"/>
+      <c r="BY1" s="104"/>
+      <c r="BZ1" s="104"/>
+      <c r="CA1" s="104"/>
+      <c r="CB1" s="104"/>
+      <c r="CC1" s="104">
         <f t="shared" ref="CC1" si="8">BV1+7</f>
         <v>42198</v>
       </c>
-      <c r="CD1" s="111"/>
-      <c r="CE1" s="111"/>
-      <c r="CF1" s="111"/>
-      <c r="CG1" s="111"/>
-      <c r="CH1" s="111"/>
-      <c r="CI1" s="111"/>
-      <c r="CJ1" s="111">
+      <c r="CD1" s="104"/>
+      <c r="CE1" s="104"/>
+      <c r="CF1" s="104"/>
+      <c r="CG1" s="104"/>
+      <c r="CH1" s="104"/>
+      <c r="CI1" s="104"/>
+      <c r="CJ1" s="104">
         <f t="shared" ref="CJ1" si="9">CC1+7</f>
         <v>42205</v>
       </c>
-      <c r="CK1" s="111"/>
-      <c r="CL1" s="111"/>
-      <c r="CM1" s="111"/>
-      <c r="CN1" s="111"/>
-      <c r="CO1" s="111"/>
-      <c r="CP1" s="111"/>
-      <c r="CQ1" s="111">
+      <c r="CK1" s="104"/>
+      <c r="CL1" s="104"/>
+      <c r="CM1" s="104"/>
+      <c r="CN1" s="104"/>
+      <c r="CO1" s="104"/>
+      <c r="CP1" s="104"/>
+      <c r="CQ1" s="104">
         <f t="shared" ref="CQ1" si="10">CJ1+7</f>
         <v>42212</v>
       </c>
-      <c r="CR1" s="111"/>
-      <c r="CS1" s="111"/>
-      <c r="CT1" s="111"/>
-      <c r="CU1" s="111"/>
-      <c r="CV1" s="111"/>
-      <c r="CW1" s="111"/>
-      <c r="CX1" s="111">
+      <c r="CR1" s="104"/>
+      <c r="CS1" s="104"/>
+      <c r="CT1" s="104"/>
+      <c r="CU1" s="104"/>
+      <c r="CV1" s="104"/>
+      <c r="CW1" s="104"/>
+      <c r="CX1" s="104">
         <f t="shared" ref="CX1" si="11">CQ1+7</f>
         <v>42219</v>
       </c>
-      <c r="CY1" s="111"/>
-      <c r="CZ1" s="111"/>
-      <c r="DA1" s="111"/>
-      <c r="DB1" s="111"/>
-      <c r="DC1" s="111"/>
-      <c r="DD1" s="111"/>
-      <c r="DE1" s="111">
+      <c r="CY1" s="104"/>
+      <c r="CZ1" s="104"/>
+      <c r="DA1" s="104"/>
+      <c r="DB1" s="104"/>
+      <c r="DC1" s="104"/>
+      <c r="DD1" s="104"/>
+      <c r="DE1" s="104">
         <f t="shared" ref="DE1" si="12">CX1+7</f>
         <v>42226</v>
       </c>
-      <c r="DF1" s="111"/>
-      <c r="DG1" s="111"/>
-      <c r="DH1" s="111"/>
-      <c r="DI1" s="111"/>
-      <c r="DJ1" s="111"/>
-      <c r="DK1" s="111"/>
-      <c r="DL1" s="111">
+      <c r="DF1" s="104"/>
+      <c r="DG1" s="104"/>
+      <c r="DH1" s="104"/>
+      <c r="DI1" s="104"/>
+      <c r="DJ1" s="104"/>
+      <c r="DK1" s="104"/>
+      <c r="DL1" s="104">
         <f t="shared" ref="DL1" si="13">DE1+7</f>
         <v>42233</v>
       </c>
-      <c r="DM1" s="111"/>
-      <c r="DN1" s="111"/>
-      <c r="DO1" s="111"/>
-      <c r="DP1" s="111"/>
-      <c r="DQ1" s="111"/>
-      <c r="DR1" s="111"/>
-      <c r="DS1" s="111">
+      <c r="DM1" s="104"/>
+      <c r="DN1" s="104"/>
+      <c r="DO1" s="104"/>
+      <c r="DP1" s="104"/>
+      <c r="DQ1" s="104"/>
+      <c r="DR1" s="104"/>
+      <c r="DS1" s="104">
         <f t="shared" ref="DS1" si="14">DL1+7</f>
         <v>42240</v>
       </c>
-      <c r="DT1" s="111"/>
-      <c r="DU1" s="111"/>
-      <c r="DV1" s="111"/>
-      <c r="DW1" s="111"/>
-      <c r="DX1" s="111"/>
-      <c r="DY1" s="111"/>
-      <c r="DZ1" s="111">
+      <c r="DT1" s="104"/>
+      <c r="DU1" s="104"/>
+      <c r="DV1" s="104"/>
+      <c r="DW1" s="104"/>
+      <c r="DX1" s="104"/>
+      <c r="DY1" s="104"/>
+      <c r="DZ1" s="104">
         <f t="shared" ref="DZ1" si="15">DS1+7</f>
         <v>42247</v>
       </c>
-      <c r="EA1" s="111"/>
-      <c r="EB1" s="111"/>
-      <c r="EC1" s="111"/>
-      <c r="ED1" s="111"/>
-      <c r="EE1" s="111"/>
-      <c r="EF1" s="111"/>
+      <c r="EA1" s="104"/>
+      <c r="EB1" s="104"/>
+      <c r="EC1" s="104"/>
+      <c r="ED1" s="104"/>
+      <c r="EE1" s="104"/>
+      <c r="EF1" s="104"/>
       <c r="EG1" s="27"/>
     </row>
     <row r="2" spans="1:137" s="9" customFormat="1" ht="34" customHeight="1" thickBot="1">
-      <c r="A2" s="110"/>
-      <c r="B2" s="108"/>
-      <c r="C2" s="110"/>
+      <c r="A2" s="111"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="111"/>
       <c r="D2" s="8" t="s">
         <v>1</v>
       </c>
@@ -3351,18 +3373,19 @@
       <c r="L10" s="24">
         <v>6</v>
       </c>
-      <c r="N10" s="34"/>
+      <c r="M10" s="113"/>
+      <c r="N10" s="113"/>
       <c r="O10" s="65"/>
       <c r="P10" s="34"/>
       <c r="Q10" s="72"/>
-      <c r="R10" s="73"/>
-      <c r="S10" s="34"/>
+      <c r="R10" s="114"/>
+      <c r="S10" s="113"/>
       <c r="T10" s="34"/>
       <c r="U10" s="77"/>
       <c r="X10" s="32"/>
-      <c r="Y10" s="12"/>
-      <c r="Z10" s="34"/>
-      <c r="AA10" s="34"/>
+      <c r="Y10" s="114"/>
+      <c r="Z10" s="113"/>
+      <c r="AA10" s="113"/>
       <c r="AB10" s="34"/>
       <c r="AC10" s="34"/>
       <c r="AD10" s="34"/>
@@ -3742,13 +3765,13 @@
       <c r="J18" s="36"/>
       <c r="K18" s="4"/>
       <c r="L18" s="35"/>
-      <c r="T18" s="104" t="s">
+      <c r="T18" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="U18" s="105"/>
-      <c r="V18" s="105"/>
-      <c r="W18" s="105"/>
-      <c r="X18" s="106"/>
+      <c r="U18" s="106"/>
+      <c r="V18" s="106"/>
+      <c r="W18" s="106"/>
+      <c r="X18" s="107"/>
       <c r="Y18" s="33">
         <v>4</v>
       </c>
@@ -3776,13 +3799,13 @@
       <c r="L19" s="34"/>
       <c r="Q19" s="32"/>
       <c r="R19" s="12"/>
-      <c r="T19" s="104" t="s">
+      <c r="T19" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="U19" s="105"/>
-      <c r="V19" s="105"/>
-      <c r="W19" s="105"/>
-      <c r="X19" s="106"/>
+      <c r="U19" s="106"/>
+      <c r="V19" s="106"/>
+      <c r="W19" s="106"/>
+      <c r="X19" s="107"/>
       <c r="Y19" s="12"/>
       <c r="Z19" s="24">
         <v>8</v>
@@ -6354,17 +6377,22 @@
       </c>
       <c r="B66" s="83"/>
     </row>
-    <row r="67" spans="1:2" ht="41" customHeight="1">
-      <c r="A67" s="14"/>
+    <row r="67" spans="1:2" ht="41" customHeight="1" thickBot="1">
+      <c r="A67" s="112" t="s">
+        <v>74</v>
+      </c>
+      <c r="B67" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="DE1:DK1"/>
-    <mergeCell ref="DL1:DR1"/>
-    <mergeCell ref="DS1:DY1"/>
-    <mergeCell ref="DZ1:EF1"/>
-    <mergeCell ref="CQ1:CW1"/>
-    <mergeCell ref="CX1:DD1"/>
+    <mergeCell ref="T19:X19"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="K1:Q1"/>
+    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="T18:X18"/>
     <mergeCell ref="BO1:BU1"/>
     <mergeCell ref="BV1:CB1"/>
     <mergeCell ref="CC1:CI1"/>
@@ -6375,14 +6403,12 @@
     <mergeCell ref="AT1:AZ1"/>
     <mergeCell ref="BA1:BG1"/>
     <mergeCell ref="BH1:BN1"/>
-    <mergeCell ref="T19:X19"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:J1"/>
-    <mergeCell ref="K1:Q1"/>
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="T18:X18"/>
+    <mergeCell ref="DE1:DK1"/>
+    <mergeCell ref="DL1:DR1"/>
+    <mergeCell ref="DS1:DY1"/>
+    <mergeCell ref="DZ1:EF1"/>
+    <mergeCell ref="CQ1:CW1"/>
+    <mergeCell ref="CX1:DD1"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
preparation vue vitals, ajout de tabs et initialisation des variables
</commit_message>
<xml_diff>
--- a/gantt-chart.xlsx
+++ b/gantt-chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16400" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="gantt" sheetId="1" r:id="rId1"/>
@@ -977,7 +977,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1288,30 +1288,6 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -1319,6 +1295,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1835,8 +1838,8 @@
   <dimension ref="A1:EG67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A67" sqref="A67"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.6640625" defaultRowHeight="41" customHeight="1" x14ac:dyDescent="0"/>
@@ -1906,210 +1909,210 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:137" s="1" customFormat="1" ht="29" customHeight="1">
-      <c r="A1" s="110" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="108" t="s">
+      <c r="A1" s="112" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="110" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="110" t="s">
+      <c r="C1" s="112" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="104">
+      <c r="D1" s="114">
         <v>42121</v>
       </c>
-      <c r="E1" s="104"/>
-      <c r="F1" s="104"/>
-      <c r="G1" s="104"/>
-      <c r="H1" s="104"/>
-      <c r="I1" s="104"/>
-      <c r="J1" s="104"/>
-      <c r="K1" s="104">
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="114">
         <f>D1+7</f>
         <v>42128</v>
       </c>
-      <c r="L1" s="104"/>
-      <c r="M1" s="104"/>
-      <c r="N1" s="104"/>
-      <c r="O1" s="104"/>
-      <c r="P1" s="104"/>
-      <c r="Q1" s="104"/>
-      <c r="R1" s="104">
+      <c r="L1" s="114"/>
+      <c r="M1" s="114"/>
+      <c r="N1" s="114"/>
+      <c r="O1" s="114"/>
+      <c r="P1" s="114"/>
+      <c r="Q1" s="114"/>
+      <c r="R1" s="114">
         <f>K1+7</f>
         <v>42135</v>
       </c>
-      <c r="S1" s="104"/>
-      <c r="T1" s="104"/>
-      <c r="U1" s="104"/>
-      <c r="V1" s="104"/>
-      <c r="W1" s="104"/>
-      <c r="X1" s="104"/>
-      <c r="Y1" s="104">
+      <c r="S1" s="114"/>
+      <c r="T1" s="114"/>
+      <c r="U1" s="114"/>
+      <c r="V1" s="114"/>
+      <c r="W1" s="114"/>
+      <c r="X1" s="114"/>
+      <c r="Y1" s="114">
         <f t="shared" ref="Y1" si="0">R1+7</f>
         <v>42142</v>
       </c>
-      <c r="Z1" s="104"/>
-      <c r="AA1" s="104"/>
-      <c r="AB1" s="104"/>
-      <c r="AC1" s="104"/>
-      <c r="AD1" s="104"/>
-      <c r="AE1" s="104"/>
-      <c r="AF1" s="104">
+      <c r="Z1" s="114"/>
+      <c r="AA1" s="114"/>
+      <c r="AB1" s="114"/>
+      <c r="AC1" s="114"/>
+      <c r="AD1" s="114"/>
+      <c r="AE1" s="114"/>
+      <c r="AF1" s="114">
         <f t="shared" ref="AF1" si="1">Y1+7</f>
         <v>42149</v>
       </c>
-      <c r="AG1" s="104"/>
-      <c r="AH1" s="104"/>
-      <c r="AI1" s="104"/>
-      <c r="AJ1" s="104"/>
-      <c r="AK1" s="104"/>
-      <c r="AL1" s="104"/>
-      <c r="AM1" s="104">
+      <c r="AG1" s="114"/>
+      <c r="AH1" s="114"/>
+      <c r="AI1" s="114"/>
+      <c r="AJ1" s="114"/>
+      <c r="AK1" s="114"/>
+      <c r="AL1" s="114"/>
+      <c r="AM1" s="114">
         <f t="shared" ref="AM1" si="2">AF1+7</f>
         <v>42156</v>
       </c>
-      <c r="AN1" s="104"/>
-      <c r="AO1" s="104"/>
-      <c r="AP1" s="104"/>
-      <c r="AQ1" s="104"/>
-      <c r="AR1" s="104"/>
-      <c r="AS1" s="104"/>
-      <c r="AT1" s="104">
+      <c r="AN1" s="114"/>
+      <c r="AO1" s="114"/>
+      <c r="AP1" s="114"/>
+      <c r="AQ1" s="114"/>
+      <c r="AR1" s="114"/>
+      <c r="AS1" s="114"/>
+      <c r="AT1" s="114">
         <f t="shared" ref="AT1" si="3">AM1+7</f>
         <v>42163</v>
       </c>
-      <c r="AU1" s="104"/>
-      <c r="AV1" s="104"/>
-      <c r="AW1" s="104"/>
-      <c r="AX1" s="104"/>
-      <c r="AY1" s="104"/>
-      <c r="AZ1" s="104"/>
-      <c r="BA1" s="104">
+      <c r="AU1" s="114"/>
+      <c r="AV1" s="114"/>
+      <c r="AW1" s="114"/>
+      <c r="AX1" s="114"/>
+      <c r="AY1" s="114"/>
+      <c r="AZ1" s="114"/>
+      <c r="BA1" s="114">
         <f t="shared" ref="BA1" si="4">AT1+7</f>
         <v>42170</v>
       </c>
-      <c r="BB1" s="104"/>
-      <c r="BC1" s="104"/>
-      <c r="BD1" s="104"/>
-      <c r="BE1" s="104"/>
-      <c r="BF1" s="104"/>
-      <c r="BG1" s="104"/>
-      <c r="BH1" s="104">
+      <c r="BB1" s="114"/>
+      <c r="BC1" s="114"/>
+      <c r="BD1" s="114"/>
+      <c r="BE1" s="114"/>
+      <c r="BF1" s="114"/>
+      <c r="BG1" s="114"/>
+      <c r="BH1" s="114">
         <f t="shared" ref="BH1" si="5">BA1+7</f>
         <v>42177</v>
       </c>
-      <c r="BI1" s="104"/>
-      <c r="BJ1" s="104"/>
-      <c r="BK1" s="104"/>
-      <c r="BL1" s="104"/>
-      <c r="BM1" s="104"/>
-      <c r="BN1" s="104"/>
-      <c r="BO1" s="104">
+      <c r="BI1" s="114"/>
+      <c r="BJ1" s="114"/>
+      <c r="BK1" s="114"/>
+      <c r="BL1" s="114"/>
+      <c r="BM1" s="114"/>
+      <c r="BN1" s="114"/>
+      <c r="BO1" s="114">
         <f t="shared" ref="BO1" si="6">BH1+7</f>
         <v>42184</v>
       </c>
-      <c r="BP1" s="104"/>
-      <c r="BQ1" s="104"/>
-      <c r="BR1" s="104"/>
-      <c r="BS1" s="104"/>
-      <c r="BT1" s="104"/>
-      <c r="BU1" s="104"/>
-      <c r="BV1" s="104">
+      <c r="BP1" s="114"/>
+      <c r="BQ1" s="114"/>
+      <c r="BR1" s="114"/>
+      <c r="BS1" s="114"/>
+      <c r="BT1" s="114"/>
+      <c r="BU1" s="114"/>
+      <c r="BV1" s="114">
         <f t="shared" ref="BV1" si="7">BO1+7</f>
         <v>42191</v>
       </c>
-      <c r="BW1" s="104"/>
-      <c r="BX1" s="104"/>
-      <c r="BY1" s="104"/>
-      <c r="BZ1" s="104"/>
-      <c r="CA1" s="104"/>
-      <c r="CB1" s="104"/>
-      <c r="CC1" s="104">
+      <c r="BW1" s="114"/>
+      <c r="BX1" s="114"/>
+      <c r="BY1" s="114"/>
+      <c r="BZ1" s="114"/>
+      <c r="CA1" s="114"/>
+      <c r="CB1" s="114"/>
+      <c r="CC1" s="114">
         <f t="shared" ref="CC1" si="8">BV1+7</f>
         <v>42198</v>
       </c>
-      <c r="CD1" s="104"/>
-      <c r="CE1" s="104"/>
-      <c r="CF1" s="104"/>
-      <c r="CG1" s="104"/>
-      <c r="CH1" s="104"/>
-      <c r="CI1" s="104"/>
-      <c r="CJ1" s="104">
+      <c r="CD1" s="114"/>
+      <c r="CE1" s="114"/>
+      <c r="CF1" s="114"/>
+      <c r="CG1" s="114"/>
+      <c r="CH1" s="114"/>
+      <c r="CI1" s="114"/>
+      <c r="CJ1" s="114">
         <f t="shared" ref="CJ1" si="9">CC1+7</f>
         <v>42205</v>
       </c>
-      <c r="CK1" s="104"/>
-      <c r="CL1" s="104"/>
-      <c r="CM1" s="104"/>
-      <c r="CN1" s="104"/>
-      <c r="CO1" s="104"/>
-      <c r="CP1" s="104"/>
-      <c r="CQ1" s="104">
+      <c r="CK1" s="114"/>
+      <c r="CL1" s="114"/>
+      <c r="CM1" s="114"/>
+      <c r="CN1" s="114"/>
+      <c r="CO1" s="114"/>
+      <c r="CP1" s="114"/>
+      <c r="CQ1" s="114">
         <f t="shared" ref="CQ1" si="10">CJ1+7</f>
         <v>42212</v>
       </c>
-      <c r="CR1" s="104"/>
-      <c r="CS1" s="104"/>
-      <c r="CT1" s="104"/>
-      <c r="CU1" s="104"/>
-      <c r="CV1" s="104"/>
-      <c r="CW1" s="104"/>
-      <c r="CX1" s="104">
+      <c r="CR1" s="114"/>
+      <c r="CS1" s="114"/>
+      <c r="CT1" s="114"/>
+      <c r="CU1" s="114"/>
+      <c r="CV1" s="114"/>
+      <c r="CW1" s="114"/>
+      <c r="CX1" s="114">
         <f t="shared" ref="CX1" si="11">CQ1+7</f>
         <v>42219</v>
       </c>
-      <c r="CY1" s="104"/>
-      <c r="CZ1" s="104"/>
-      <c r="DA1" s="104"/>
-      <c r="DB1" s="104"/>
-      <c r="DC1" s="104"/>
-      <c r="DD1" s="104"/>
-      <c r="DE1" s="104">
+      <c r="CY1" s="114"/>
+      <c r="CZ1" s="114"/>
+      <c r="DA1" s="114"/>
+      <c r="DB1" s="114"/>
+      <c r="DC1" s="114"/>
+      <c r="DD1" s="114"/>
+      <c r="DE1" s="114">
         <f t="shared" ref="DE1" si="12">CX1+7</f>
         <v>42226</v>
       </c>
-      <c r="DF1" s="104"/>
-      <c r="DG1" s="104"/>
-      <c r="DH1" s="104"/>
-      <c r="DI1" s="104"/>
-      <c r="DJ1" s="104"/>
-      <c r="DK1" s="104"/>
-      <c r="DL1" s="104">
+      <c r="DF1" s="114"/>
+      <c r="DG1" s="114"/>
+      <c r="DH1" s="114"/>
+      <c r="DI1" s="114"/>
+      <c r="DJ1" s="114"/>
+      <c r="DK1" s="114"/>
+      <c r="DL1" s="114">
         <f t="shared" ref="DL1" si="13">DE1+7</f>
         <v>42233</v>
       </c>
-      <c r="DM1" s="104"/>
-      <c r="DN1" s="104"/>
-      <c r="DO1" s="104"/>
-      <c r="DP1" s="104"/>
-      <c r="DQ1" s="104"/>
-      <c r="DR1" s="104"/>
-      <c r="DS1" s="104">
+      <c r="DM1" s="114"/>
+      <c r="DN1" s="114"/>
+      <c r="DO1" s="114"/>
+      <c r="DP1" s="114"/>
+      <c r="DQ1" s="114"/>
+      <c r="DR1" s="114"/>
+      <c r="DS1" s="114">
         <f t="shared" ref="DS1" si="14">DL1+7</f>
         <v>42240</v>
       </c>
-      <c r="DT1" s="104"/>
-      <c r="DU1" s="104"/>
-      <c r="DV1" s="104"/>
-      <c r="DW1" s="104"/>
-      <c r="DX1" s="104"/>
-      <c r="DY1" s="104"/>
-      <c r="DZ1" s="104">
+      <c r="DT1" s="114"/>
+      <c r="DU1" s="114"/>
+      <c r="DV1" s="114"/>
+      <c r="DW1" s="114"/>
+      <c r="DX1" s="114"/>
+      <c r="DY1" s="114"/>
+      <c r="DZ1" s="114">
         <f t="shared" ref="DZ1" si="15">DS1+7</f>
         <v>42247</v>
       </c>
-      <c r="EA1" s="104"/>
-      <c r="EB1" s="104"/>
-      <c r="EC1" s="104"/>
-      <c r="ED1" s="104"/>
-      <c r="EE1" s="104"/>
-      <c r="EF1" s="104"/>
+      <c r="EA1" s="114"/>
+      <c r="EB1" s="114"/>
+      <c r="EC1" s="114"/>
+      <c r="ED1" s="114"/>
+      <c r="EE1" s="114"/>
+      <c r="EF1" s="114"/>
       <c r="EG1" s="27"/>
     </row>
     <row r="2" spans="1:137" s="9" customFormat="1" ht="34" customHeight="1" thickBot="1">
-      <c r="A2" s="111"/>
-      <c r="B2" s="109"/>
-      <c r="C2" s="111"/>
+      <c r="A2" s="113"/>
+      <c r="B2" s="111"/>
+      <c r="C2" s="113"/>
       <c r="D2" s="8" t="s">
         <v>1</v>
       </c>
@@ -3370,22 +3373,22 @@
       <c r="K10" s="101">
         <v>6</v>
       </c>
-      <c r="L10" s="24">
+      <c r="L10" s="100">
         <v>6</v>
       </c>
-      <c r="M10" s="113"/>
-      <c r="N10" s="113"/>
+      <c r="M10" s="105"/>
+      <c r="N10" s="105"/>
       <c r="O10" s="65"/>
       <c r="P10" s="34"/>
       <c r="Q10" s="72"/>
-      <c r="R10" s="114"/>
-      <c r="S10" s="113"/>
+      <c r="R10" s="106"/>
+      <c r="S10" s="105"/>
       <c r="T10" s="34"/>
       <c r="U10" s="77"/>
       <c r="X10" s="32"/>
-      <c r="Y10" s="114"/>
-      <c r="Z10" s="113"/>
-      <c r="AA10" s="113"/>
+      <c r="Y10" s="106"/>
+      <c r="Z10" s="105"/>
+      <c r="AA10" s="105"/>
       <c r="AB10" s="34"/>
       <c r="AC10" s="34"/>
       <c r="AD10" s="34"/>
@@ -3557,7 +3560,7 @@
       <c r="J13" s="36"/>
       <c r="K13" s="35"/>
       <c r="L13" s="35"/>
-      <c r="M13" s="23">
+      <c r="M13" s="99">
         <v>6</v>
       </c>
       <c r="N13" s="25">
@@ -3570,6 +3573,7 @@
       <c r="S13" s="35"/>
       <c r="T13" s="35"/>
       <c r="U13" s="35"/>
+      <c r="AB13" s="115"/>
     </row>
     <row r="14" spans="1:137" ht="41" customHeight="1">
       <c r="A14" s="6" t="s">
@@ -3599,6 +3603,7 @@
       <c r="S14" s="22"/>
       <c r="T14" s="35"/>
       <c r="U14" s="35"/>
+      <c r="AB14" s="115"/>
     </row>
     <row r="15" spans="1:137" ht="41" customHeight="1">
       <c r="A15" s="6" t="s">
@@ -3628,6 +3633,7 @@
       <c r="S15" s="37"/>
       <c r="T15" s="64"/>
       <c r="U15" s="35"/>
+      <c r="AB15" s="115"/>
     </row>
     <row r="16" spans="1:137" s="13" customFormat="1" ht="41" customHeight="1" thickBot="1">
       <c r="A16" s="10" t="s">
@@ -3765,13 +3771,13 @@
       <c r="J18" s="36"/>
       <c r="K18" s="4"/>
       <c r="L18" s="35"/>
-      <c r="T18" s="105" t="s">
+      <c r="T18" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="U18" s="106"/>
-      <c r="V18" s="106"/>
-      <c r="W18" s="106"/>
-      <c r="X18" s="107"/>
+      <c r="U18" s="108"/>
+      <c r="V18" s="108"/>
+      <c r="W18" s="108"/>
+      <c r="X18" s="109"/>
       <c r="Y18" s="33">
         <v>4</v>
       </c>
@@ -3799,13 +3805,13 @@
       <c r="L19" s="34"/>
       <c r="Q19" s="32"/>
       <c r="R19" s="12"/>
-      <c r="T19" s="105" t="s">
+      <c r="T19" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="U19" s="106"/>
-      <c r="V19" s="106"/>
-      <c r="W19" s="106"/>
-      <c r="X19" s="107"/>
+      <c r="U19" s="108"/>
+      <c r="V19" s="108"/>
+      <c r="W19" s="108"/>
+      <c r="X19" s="109"/>
       <c r="Y19" s="12"/>
       <c r="Z19" s="24">
         <v>8</v>
@@ -6378,21 +6384,19 @@
       <c r="B66" s="83"/>
     </row>
     <row r="67" spans="1:2" ht="41" customHeight="1" thickBot="1">
-      <c r="A67" s="112" t="s">
+      <c r="A67" s="104" t="s">
         <v>74</v>
       </c>
       <c r="B67" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="T19:X19"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:J1"/>
-    <mergeCell ref="K1:Q1"/>
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="T18:X18"/>
+    <mergeCell ref="DE1:DK1"/>
+    <mergeCell ref="DL1:DR1"/>
+    <mergeCell ref="DS1:DY1"/>
+    <mergeCell ref="DZ1:EF1"/>
+    <mergeCell ref="CQ1:CW1"/>
+    <mergeCell ref="CX1:DD1"/>
     <mergeCell ref="BO1:BU1"/>
     <mergeCell ref="BV1:CB1"/>
     <mergeCell ref="CC1:CI1"/>
@@ -6403,12 +6407,14 @@
     <mergeCell ref="AT1:AZ1"/>
     <mergeCell ref="BA1:BG1"/>
     <mergeCell ref="BH1:BN1"/>
-    <mergeCell ref="DE1:DK1"/>
-    <mergeCell ref="DL1:DR1"/>
-    <mergeCell ref="DS1:DY1"/>
-    <mergeCell ref="DZ1:EF1"/>
-    <mergeCell ref="CQ1:CW1"/>
-    <mergeCell ref="CX1:DD1"/>
+    <mergeCell ref="T19:X19"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="K1:Q1"/>
+    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="T18:X18"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
view vitals functionnal + view hitoric of vitals measure created and accessible via double tap on the preview
</commit_message>
<xml_diff>
--- a/gantt-chart.xlsx
+++ b/gantt-chart.xlsx
@@ -1297,6 +1297,12 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1316,12 +1322,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1838,8 +1838,8 @@
   <dimension ref="A1:EG67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.6640625" defaultRowHeight="41" customHeight="1" x14ac:dyDescent="0"/>
@@ -1909,210 +1909,210 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:137" s="1" customFormat="1" ht="29" customHeight="1">
-      <c r="A1" s="112" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="110" t="s">
+      <c r="A1" s="114" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="112" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="112" t="s">
+      <c r="C1" s="114" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="114">
+      <c r="D1" s="108">
         <v>42121</v>
       </c>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
-      <c r="J1" s="114"/>
-      <c r="K1" s="114">
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="108"/>
+      <c r="I1" s="108"/>
+      <c r="J1" s="108"/>
+      <c r="K1" s="108">
         <f>D1+7</f>
         <v>42128</v>
       </c>
-      <c r="L1" s="114"/>
-      <c r="M1" s="114"/>
-      <c r="N1" s="114"/>
-      <c r="O1" s="114"/>
-      <c r="P1" s="114"/>
-      <c r="Q1" s="114"/>
-      <c r="R1" s="114">
+      <c r="L1" s="108"/>
+      <c r="M1" s="108"/>
+      <c r="N1" s="108"/>
+      <c r="O1" s="108"/>
+      <c r="P1" s="108"/>
+      <c r="Q1" s="108"/>
+      <c r="R1" s="108">
         <f>K1+7</f>
         <v>42135</v>
       </c>
-      <c r="S1" s="114"/>
-      <c r="T1" s="114"/>
-      <c r="U1" s="114"/>
-      <c r="V1" s="114"/>
-      <c r="W1" s="114"/>
-      <c r="X1" s="114"/>
-      <c r="Y1" s="114">
+      <c r="S1" s="108"/>
+      <c r="T1" s="108"/>
+      <c r="U1" s="108"/>
+      <c r="V1" s="108"/>
+      <c r="W1" s="108"/>
+      <c r="X1" s="108"/>
+      <c r="Y1" s="108">
         <f t="shared" ref="Y1" si="0">R1+7</f>
         <v>42142</v>
       </c>
-      <c r="Z1" s="114"/>
-      <c r="AA1" s="114"/>
-      <c r="AB1" s="114"/>
-      <c r="AC1" s="114"/>
-      <c r="AD1" s="114"/>
-      <c r="AE1" s="114"/>
-      <c r="AF1" s="114">
+      <c r="Z1" s="108"/>
+      <c r="AA1" s="108"/>
+      <c r="AB1" s="108"/>
+      <c r="AC1" s="108"/>
+      <c r="AD1" s="108"/>
+      <c r="AE1" s="108"/>
+      <c r="AF1" s="108">
         <f t="shared" ref="AF1" si="1">Y1+7</f>
         <v>42149</v>
       </c>
-      <c r="AG1" s="114"/>
-      <c r="AH1" s="114"/>
-      <c r="AI1" s="114"/>
-      <c r="AJ1" s="114"/>
-      <c r="AK1" s="114"/>
-      <c r="AL1" s="114"/>
-      <c r="AM1" s="114">
+      <c r="AG1" s="108"/>
+      <c r="AH1" s="108"/>
+      <c r="AI1" s="108"/>
+      <c r="AJ1" s="108"/>
+      <c r="AK1" s="108"/>
+      <c r="AL1" s="108"/>
+      <c r="AM1" s="108">
         <f t="shared" ref="AM1" si="2">AF1+7</f>
         <v>42156</v>
       </c>
-      <c r="AN1" s="114"/>
-      <c r="AO1" s="114"/>
-      <c r="AP1" s="114"/>
-      <c r="AQ1" s="114"/>
-      <c r="AR1" s="114"/>
-      <c r="AS1" s="114"/>
-      <c r="AT1" s="114">
+      <c r="AN1" s="108"/>
+      <c r="AO1" s="108"/>
+      <c r="AP1" s="108"/>
+      <c r="AQ1" s="108"/>
+      <c r="AR1" s="108"/>
+      <c r="AS1" s="108"/>
+      <c r="AT1" s="108">
         <f t="shared" ref="AT1" si="3">AM1+7</f>
         <v>42163</v>
       </c>
-      <c r="AU1" s="114"/>
-      <c r="AV1" s="114"/>
-      <c r="AW1" s="114"/>
-      <c r="AX1" s="114"/>
-      <c r="AY1" s="114"/>
-      <c r="AZ1" s="114"/>
-      <c r="BA1" s="114">
+      <c r="AU1" s="108"/>
+      <c r="AV1" s="108"/>
+      <c r="AW1" s="108"/>
+      <c r="AX1" s="108"/>
+      <c r="AY1" s="108"/>
+      <c r="AZ1" s="108"/>
+      <c r="BA1" s="108">
         <f t="shared" ref="BA1" si="4">AT1+7</f>
         <v>42170</v>
       </c>
-      <c r="BB1" s="114"/>
-      <c r="BC1" s="114"/>
-      <c r="BD1" s="114"/>
-      <c r="BE1" s="114"/>
-      <c r="BF1" s="114"/>
-      <c r="BG1" s="114"/>
-      <c r="BH1" s="114">
+      <c r="BB1" s="108"/>
+      <c r="BC1" s="108"/>
+      <c r="BD1" s="108"/>
+      <c r="BE1" s="108"/>
+      <c r="BF1" s="108"/>
+      <c r="BG1" s="108"/>
+      <c r="BH1" s="108">
         <f t="shared" ref="BH1" si="5">BA1+7</f>
         <v>42177</v>
       </c>
-      <c r="BI1" s="114"/>
-      <c r="BJ1" s="114"/>
-      <c r="BK1" s="114"/>
-      <c r="BL1" s="114"/>
-      <c r="BM1" s="114"/>
-      <c r="BN1" s="114"/>
-      <c r="BO1" s="114">
+      <c r="BI1" s="108"/>
+      <c r="BJ1" s="108"/>
+      <c r="BK1" s="108"/>
+      <c r="BL1" s="108"/>
+      <c r="BM1" s="108"/>
+      <c r="BN1" s="108"/>
+      <c r="BO1" s="108">
         <f t="shared" ref="BO1" si="6">BH1+7</f>
         <v>42184</v>
       </c>
-      <c r="BP1" s="114"/>
-      <c r="BQ1" s="114"/>
-      <c r="BR1" s="114"/>
-      <c r="BS1" s="114"/>
-      <c r="BT1" s="114"/>
-      <c r="BU1" s="114"/>
-      <c r="BV1" s="114">
+      <c r="BP1" s="108"/>
+      <c r="BQ1" s="108"/>
+      <c r="BR1" s="108"/>
+      <c r="BS1" s="108"/>
+      <c r="BT1" s="108"/>
+      <c r="BU1" s="108"/>
+      <c r="BV1" s="108">
         <f t="shared" ref="BV1" si="7">BO1+7</f>
         <v>42191</v>
       </c>
-      <c r="BW1" s="114"/>
-      <c r="BX1" s="114"/>
-      <c r="BY1" s="114"/>
-      <c r="BZ1" s="114"/>
-      <c r="CA1" s="114"/>
-      <c r="CB1" s="114"/>
-      <c r="CC1" s="114">
+      <c r="BW1" s="108"/>
+      <c r="BX1" s="108"/>
+      <c r="BY1" s="108"/>
+      <c r="BZ1" s="108"/>
+      <c r="CA1" s="108"/>
+      <c r="CB1" s="108"/>
+      <c r="CC1" s="108">
         <f t="shared" ref="CC1" si="8">BV1+7</f>
         <v>42198</v>
       </c>
-      <c r="CD1" s="114"/>
-      <c r="CE1" s="114"/>
-      <c r="CF1" s="114"/>
-      <c r="CG1" s="114"/>
-      <c r="CH1" s="114"/>
-      <c r="CI1" s="114"/>
-      <c r="CJ1" s="114">
+      <c r="CD1" s="108"/>
+      <c r="CE1" s="108"/>
+      <c r="CF1" s="108"/>
+      <c r="CG1" s="108"/>
+      <c r="CH1" s="108"/>
+      <c r="CI1" s="108"/>
+      <c r="CJ1" s="108">
         <f t="shared" ref="CJ1" si="9">CC1+7</f>
         <v>42205</v>
       </c>
-      <c r="CK1" s="114"/>
-      <c r="CL1" s="114"/>
-      <c r="CM1" s="114"/>
-      <c r="CN1" s="114"/>
-      <c r="CO1" s="114"/>
-      <c r="CP1" s="114"/>
-      <c r="CQ1" s="114">
+      <c r="CK1" s="108"/>
+      <c r="CL1" s="108"/>
+      <c r="CM1" s="108"/>
+      <c r="CN1" s="108"/>
+      <c r="CO1" s="108"/>
+      <c r="CP1" s="108"/>
+      <c r="CQ1" s="108">
         <f t="shared" ref="CQ1" si="10">CJ1+7</f>
         <v>42212</v>
       </c>
-      <c r="CR1" s="114"/>
-      <c r="CS1" s="114"/>
-      <c r="CT1" s="114"/>
-      <c r="CU1" s="114"/>
-      <c r="CV1" s="114"/>
-      <c r="CW1" s="114"/>
-      <c r="CX1" s="114">
+      <c r="CR1" s="108"/>
+      <c r="CS1" s="108"/>
+      <c r="CT1" s="108"/>
+      <c r="CU1" s="108"/>
+      <c r="CV1" s="108"/>
+      <c r="CW1" s="108"/>
+      <c r="CX1" s="108">
         <f t="shared" ref="CX1" si="11">CQ1+7</f>
         <v>42219</v>
       </c>
-      <c r="CY1" s="114"/>
-      <c r="CZ1" s="114"/>
-      <c r="DA1" s="114"/>
-      <c r="DB1" s="114"/>
-      <c r="DC1" s="114"/>
-      <c r="DD1" s="114"/>
-      <c r="DE1" s="114">
+      <c r="CY1" s="108"/>
+      <c r="CZ1" s="108"/>
+      <c r="DA1" s="108"/>
+      <c r="DB1" s="108"/>
+      <c r="DC1" s="108"/>
+      <c r="DD1" s="108"/>
+      <c r="DE1" s="108">
         <f t="shared" ref="DE1" si="12">CX1+7</f>
         <v>42226</v>
       </c>
-      <c r="DF1" s="114"/>
-      <c r="DG1" s="114"/>
-      <c r="DH1" s="114"/>
-      <c r="DI1" s="114"/>
-      <c r="DJ1" s="114"/>
-      <c r="DK1" s="114"/>
-      <c r="DL1" s="114">
+      <c r="DF1" s="108"/>
+      <c r="DG1" s="108"/>
+      <c r="DH1" s="108"/>
+      <c r="DI1" s="108"/>
+      <c r="DJ1" s="108"/>
+      <c r="DK1" s="108"/>
+      <c r="DL1" s="108">
         <f t="shared" ref="DL1" si="13">DE1+7</f>
         <v>42233</v>
       </c>
-      <c r="DM1" s="114"/>
-      <c r="DN1" s="114"/>
-      <c r="DO1" s="114"/>
-      <c r="DP1" s="114"/>
-      <c r="DQ1" s="114"/>
-      <c r="DR1" s="114"/>
-      <c r="DS1" s="114">
+      <c r="DM1" s="108"/>
+      <c r="DN1" s="108"/>
+      <c r="DO1" s="108"/>
+      <c r="DP1" s="108"/>
+      <c r="DQ1" s="108"/>
+      <c r="DR1" s="108"/>
+      <c r="DS1" s="108">
         <f t="shared" ref="DS1" si="14">DL1+7</f>
         <v>42240</v>
       </c>
-      <c r="DT1" s="114"/>
-      <c r="DU1" s="114"/>
-      <c r="DV1" s="114"/>
-      <c r="DW1" s="114"/>
-      <c r="DX1" s="114"/>
-      <c r="DY1" s="114"/>
-      <c r="DZ1" s="114">
+      <c r="DT1" s="108"/>
+      <c r="DU1" s="108"/>
+      <c r="DV1" s="108"/>
+      <c r="DW1" s="108"/>
+      <c r="DX1" s="108"/>
+      <c r="DY1" s="108"/>
+      <c r="DZ1" s="108">
         <f t="shared" ref="DZ1" si="15">DS1+7</f>
         <v>42247</v>
       </c>
-      <c r="EA1" s="114"/>
-      <c r="EB1" s="114"/>
-      <c r="EC1" s="114"/>
-      <c r="ED1" s="114"/>
-      <c r="EE1" s="114"/>
-      <c r="EF1" s="114"/>
+      <c r="EA1" s="108"/>
+      <c r="EB1" s="108"/>
+      <c r="EC1" s="108"/>
+      <c r="ED1" s="108"/>
+      <c r="EE1" s="108"/>
+      <c r="EF1" s="108"/>
       <c r="EG1" s="27"/>
     </row>
     <row r="2" spans="1:137" s="9" customFormat="1" ht="34" customHeight="1" thickBot="1">
-      <c r="A2" s="113"/>
-      <c r="B2" s="111"/>
-      <c r="C2" s="113"/>
+      <c r="A2" s="115"/>
+      <c r="B2" s="113"/>
+      <c r="C2" s="115"/>
       <c r="D2" s="8" t="s">
         <v>1</v>
       </c>
@@ -3573,7 +3573,7 @@
       <c r="S13" s="35"/>
       <c r="T13" s="35"/>
       <c r="U13" s="35"/>
-      <c r="AB13" s="115"/>
+      <c r="AB13" s="107"/>
     </row>
     <row r="14" spans="1:137" ht="41" customHeight="1">
       <c r="A14" s="6" t="s">
@@ -3603,7 +3603,7 @@
       <c r="S14" s="22"/>
       <c r="T14" s="35"/>
       <c r="U14" s="35"/>
-      <c r="AB14" s="115"/>
+      <c r="AB14" s="107"/>
     </row>
     <row r="15" spans="1:137" ht="41" customHeight="1">
       <c r="A15" s="6" t="s">
@@ -3627,13 +3627,13 @@
       <c r="O15" s="35"/>
       <c r="P15" s="35"/>
       <c r="Q15" s="36"/>
-      <c r="R15" s="33">
+      <c r="R15" s="102">
         <v>6</v>
       </c>
       <c r="S15" s="37"/>
       <c r="T15" s="64"/>
       <c r="U15" s="35"/>
-      <c r="AB15" s="115"/>
+      <c r="AB15" s="107"/>
     </row>
     <row r="16" spans="1:137" s="13" customFormat="1" ht="41" customHeight="1" thickBot="1">
       <c r="A16" s="10" t="s">
@@ -3659,13 +3659,14 @@
       <c r="P16" s="34"/>
       <c r="Q16" s="72"/>
       <c r="R16" s="73"/>
-      <c r="S16" s="24">
+      <c r="S16" s="100">
         <v>4</v>
       </c>
       <c r="T16" s="37"/>
       <c r="U16" s="65"/>
       <c r="X16" s="32"/>
       <c r="Y16" s="12"/>
+      <c r="AC16" s="105"/>
       <c r="AE16" s="32"/>
       <c r="AF16" s="12"/>
       <c r="AL16" s="32"/>
@@ -3771,13 +3772,13 @@
       <c r="J18" s="36"/>
       <c r="K18" s="4"/>
       <c r="L18" s="35"/>
-      <c r="T18" s="107" t="s">
+      <c r="T18" s="109" t="s">
         <v>12</v>
       </c>
-      <c r="U18" s="108"/>
-      <c r="V18" s="108"/>
-      <c r="W18" s="108"/>
-      <c r="X18" s="109"/>
+      <c r="U18" s="110"/>
+      <c r="V18" s="110"/>
+      <c r="W18" s="110"/>
+      <c r="X18" s="111"/>
       <c r="Y18" s="33">
         <v>4</v>
       </c>
@@ -3805,13 +3806,13 @@
       <c r="L19" s="34"/>
       <c r="Q19" s="32"/>
       <c r="R19" s="12"/>
-      <c r="T19" s="107" t="s">
+      <c r="T19" s="109" t="s">
         <v>12</v>
       </c>
-      <c r="U19" s="108"/>
-      <c r="V19" s="108"/>
-      <c r="W19" s="108"/>
-      <c r="X19" s="109"/>
+      <c r="U19" s="110"/>
+      <c r="V19" s="110"/>
+      <c r="W19" s="110"/>
+      <c r="X19" s="111"/>
       <c r="Y19" s="12"/>
       <c r="Z19" s="24">
         <v>8</v>
@@ -6391,12 +6392,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="DE1:DK1"/>
-    <mergeCell ref="DL1:DR1"/>
-    <mergeCell ref="DS1:DY1"/>
-    <mergeCell ref="DZ1:EF1"/>
-    <mergeCell ref="CQ1:CW1"/>
-    <mergeCell ref="CX1:DD1"/>
+    <mergeCell ref="T19:X19"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="K1:Q1"/>
+    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="T18:X18"/>
     <mergeCell ref="BO1:BU1"/>
     <mergeCell ref="BV1:CB1"/>
     <mergeCell ref="CC1:CI1"/>
@@ -6407,14 +6410,12 @@
     <mergeCell ref="AT1:AZ1"/>
     <mergeCell ref="BA1:BG1"/>
     <mergeCell ref="BH1:BN1"/>
-    <mergeCell ref="T19:X19"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:J1"/>
-    <mergeCell ref="K1:Q1"/>
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="T18:X18"/>
+    <mergeCell ref="DE1:DK1"/>
+    <mergeCell ref="DL1:DR1"/>
+    <mergeCell ref="DS1:DY1"/>
+    <mergeCell ref="DZ1:EF1"/>
+    <mergeCell ref="CQ1:CW1"/>
+    <mergeCell ref="CX1:DD1"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
app almost finished still needs some additional info from Mr. Ehrler to finalize it, IBeacon still doesn't work
</commit_message>
<xml_diff>
--- a/gantt-chart.xlsx
+++ b/gantt-chart.xlsx
@@ -317,7 +317,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -414,6 +414,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="29">
     <border>
@@ -977,7 +983,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1249,9 +1255,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1300,28 +1303,43 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1837,9 +1855,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EG67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X36" sqref="X36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.6640625" defaultRowHeight="41" customHeight="1" x14ac:dyDescent="0"/>
@@ -1909,210 +1927,210 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:137" s="1" customFormat="1" ht="29" customHeight="1">
-      <c r="A1" s="114" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="112" t="s">
+      <c r="A1" s="117" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="115" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="114" t="s">
+      <c r="C1" s="117" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="108">
+      <c r="D1" s="119">
         <v>42121</v>
       </c>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
-      <c r="G1" s="108"/>
-      <c r="H1" s="108"/>
-      <c r="I1" s="108"/>
-      <c r="J1" s="108"/>
-      <c r="K1" s="108">
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="119"/>
+      <c r="I1" s="119"/>
+      <c r="J1" s="119"/>
+      <c r="K1" s="119">
         <f>D1+7</f>
         <v>42128</v>
       </c>
-      <c r="L1" s="108"/>
-      <c r="M1" s="108"/>
-      <c r="N1" s="108"/>
-      <c r="O1" s="108"/>
-      <c r="P1" s="108"/>
-      <c r="Q1" s="108"/>
-      <c r="R1" s="108">
+      <c r="L1" s="119"/>
+      <c r="M1" s="119"/>
+      <c r="N1" s="119"/>
+      <c r="O1" s="119"/>
+      <c r="P1" s="119"/>
+      <c r="Q1" s="119"/>
+      <c r="R1" s="119">
         <f>K1+7</f>
         <v>42135</v>
       </c>
-      <c r="S1" s="108"/>
-      <c r="T1" s="108"/>
-      <c r="U1" s="108"/>
-      <c r="V1" s="108"/>
-      <c r="W1" s="108"/>
-      <c r="X1" s="108"/>
-      <c r="Y1" s="108">
+      <c r="S1" s="119"/>
+      <c r="T1" s="119"/>
+      <c r="U1" s="119"/>
+      <c r="V1" s="119"/>
+      <c r="W1" s="119"/>
+      <c r="X1" s="119"/>
+      <c r="Y1" s="119">
         <f t="shared" ref="Y1" si="0">R1+7</f>
         <v>42142</v>
       </c>
-      <c r="Z1" s="108"/>
-      <c r="AA1" s="108"/>
-      <c r="AB1" s="108"/>
-      <c r="AC1" s="108"/>
-      <c r="AD1" s="108"/>
-      <c r="AE1" s="108"/>
-      <c r="AF1" s="108">
+      <c r="Z1" s="119"/>
+      <c r="AA1" s="119"/>
+      <c r="AB1" s="119"/>
+      <c r="AC1" s="119"/>
+      <c r="AD1" s="119"/>
+      <c r="AE1" s="119"/>
+      <c r="AF1" s="119">
         <f t="shared" ref="AF1" si="1">Y1+7</f>
         <v>42149</v>
       </c>
-      <c r="AG1" s="108"/>
-      <c r="AH1" s="108"/>
-      <c r="AI1" s="108"/>
-      <c r="AJ1" s="108"/>
-      <c r="AK1" s="108"/>
-      <c r="AL1" s="108"/>
-      <c r="AM1" s="108">
+      <c r="AG1" s="119"/>
+      <c r="AH1" s="119"/>
+      <c r="AI1" s="119"/>
+      <c r="AJ1" s="119"/>
+      <c r="AK1" s="119"/>
+      <c r="AL1" s="119"/>
+      <c r="AM1" s="119">
         <f t="shared" ref="AM1" si="2">AF1+7</f>
         <v>42156</v>
       </c>
-      <c r="AN1" s="108"/>
-      <c r="AO1" s="108"/>
-      <c r="AP1" s="108"/>
-      <c r="AQ1" s="108"/>
-      <c r="AR1" s="108"/>
-      <c r="AS1" s="108"/>
-      <c r="AT1" s="108">
+      <c r="AN1" s="119"/>
+      <c r="AO1" s="119"/>
+      <c r="AP1" s="119"/>
+      <c r="AQ1" s="119"/>
+      <c r="AR1" s="119"/>
+      <c r="AS1" s="119"/>
+      <c r="AT1" s="119">
         <f t="shared" ref="AT1" si="3">AM1+7</f>
         <v>42163</v>
       </c>
-      <c r="AU1" s="108"/>
-      <c r="AV1" s="108"/>
-      <c r="AW1" s="108"/>
-      <c r="AX1" s="108"/>
-      <c r="AY1" s="108"/>
-      <c r="AZ1" s="108"/>
-      <c r="BA1" s="108">
+      <c r="AU1" s="119"/>
+      <c r="AV1" s="119"/>
+      <c r="AW1" s="119"/>
+      <c r="AX1" s="119"/>
+      <c r="AY1" s="119"/>
+      <c r="AZ1" s="119"/>
+      <c r="BA1" s="119">
         <f t="shared" ref="BA1" si="4">AT1+7</f>
         <v>42170</v>
       </c>
-      <c r="BB1" s="108"/>
-      <c r="BC1" s="108"/>
-      <c r="BD1" s="108"/>
-      <c r="BE1" s="108"/>
-      <c r="BF1" s="108"/>
-      <c r="BG1" s="108"/>
-      <c r="BH1" s="108">
+      <c r="BB1" s="119"/>
+      <c r="BC1" s="119"/>
+      <c r="BD1" s="119"/>
+      <c r="BE1" s="119"/>
+      <c r="BF1" s="119"/>
+      <c r="BG1" s="119"/>
+      <c r="BH1" s="119">
         <f t="shared" ref="BH1" si="5">BA1+7</f>
         <v>42177</v>
       </c>
-      <c r="BI1" s="108"/>
-      <c r="BJ1" s="108"/>
-      <c r="BK1" s="108"/>
-      <c r="BL1" s="108"/>
-      <c r="BM1" s="108"/>
-      <c r="BN1" s="108"/>
-      <c r="BO1" s="108">
+      <c r="BI1" s="119"/>
+      <c r="BJ1" s="119"/>
+      <c r="BK1" s="119"/>
+      <c r="BL1" s="119"/>
+      <c r="BM1" s="119"/>
+      <c r="BN1" s="119"/>
+      <c r="BO1" s="119">
         <f t="shared" ref="BO1" si="6">BH1+7</f>
         <v>42184</v>
       </c>
-      <c r="BP1" s="108"/>
-      <c r="BQ1" s="108"/>
-      <c r="BR1" s="108"/>
-      <c r="BS1" s="108"/>
-      <c r="BT1" s="108"/>
-      <c r="BU1" s="108"/>
-      <c r="BV1" s="108">
+      <c r="BP1" s="119"/>
+      <c r="BQ1" s="119"/>
+      <c r="BR1" s="119"/>
+      <c r="BS1" s="119"/>
+      <c r="BT1" s="119"/>
+      <c r="BU1" s="119"/>
+      <c r="BV1" s="119">
         <f t="shared" ref="BV1" si="7">BO1+7</f>
         <v>42191</v>
       </c>
-      <c r="BW1" s="108"/>
-      <c r="BX1" s="108"/>
-      <c r="BY1" s="108"/>
-      <c r="BZ1" s="108"/>
-      <c r="CA1" s="108"/>
-      <c r="CB1" s="108"/>
-      <c r="CC1" s="108">
+      <c r="BW1" s="119"/>
+      <c r="BX1" s="119"/>
+      <c r="BY1" s="119"/>
+      <c r="BZ1" s="119"/>
+      <c r="CA1" s="119"/>
+      <c r="CB1" s="119"/>
+      <c r="CC1" s="119">
         <f t="shared" ref="CC1" si="8">BV1+7</f>
         <v>42198</v>
       </c>
-      <c r="CD1" s="108"/>
-      <c r="CE1" s="108"/>
-      <c r="CF1" s="108"/>
-      <c r="CG1" s="108"/>
-      <c r="CH1" s="108"/>
-      <c r="CI1" s="108"/>
-      <c r="CJ1" s="108">
+      <c r="CD1" s="119"/>
+      <c r="CE1" s="119"/>
+      <c r="CF1" s="119"/>
+      <c r="CG1" s="119"/>
+      <c r="CH1" s="119"/>
+      <c r="CI1" s="119"/>
+      <c r="CJ1" s="119">
         <f t="shared" ref="CJ1" si="9">CC1+7</f>
         <v>42205</v>
       </c>
-      <c r="CK1" s="108"/>
-      <c r="CL1" s="108"/>
-      <c r="CM1" s="108"/>
-      <c r="CN1" s="108"/>
-      <c r="CO1" s="108"/>
-      <c r="CP1" s="108"/>
-      <c r="CQ1" s="108">
+      <c r="CK1" s="119"/>
+      <c r="CL1" s="119"/>
+      <c r="CM1" s="119"/>
+      <c r="CN1" s="119"/>
+      <c r="CO1" s="119"/>
+      <c r="CP1" s="119"/>
+      <c r="CQ1" s="119">
         <f t="shared" ref="CQ1" si="10">CJ1+7</f>
         <v>42212</v>
       </c>
-      <c r="CR1" s="108"/>
-      <c r="CS1" s="108"/>
-      <c r="CT1" s="108"/>
-      <c r="CU1" s="108"/>
-      <c r="CV1" s="108"/>
-      <c r="CW1" s="108"/>
-      <c r="CX1" s="108">
+      <c r="CR1" s="119"/>
+      <c r="CS1" s="119"/>
+      <c r="CT1" s="119"/>
+      <c r="CU1" s="119"/>
+      <c r="CV1" s="119"/>
+      <c r="CW1" s="119"/>
+      <c r="CX1" s="119">
         <f t="shared" ref="CX1" si="11">CQ1+7</f>
         <v>42219</v>
       </c>
-      <c r="CY1" s="108"/>
-      <c r="CZ1" s="108"/>
-      <c r="DA1" s="108"/>
-      <c r="DB1" s="108"/>
-      <c r="DC1" s="108"/>
-      <c r="DD1" s="108"/>
-      <c r="DE1" s="108">
+      <c r="CY1" s="119"/>
+      <c r="CZ1" s="119"/>
+      <c r="DA1" s="119"/>
+      <c r="DB1" s="119"/>
+      <c r="DC1" s="119"/>
+      <c r="DD1" s="119"/>
+      <c r="DE1" s="119">
         <f t="shared" ref="DE1" si="12">CX1+7</f>
         <v>42226</v>
       </c>
-      <c r="DF1" s="108"/>
-      <c r="DG1" s="108"/>
-      <c r="DH1" s="108"/>
-      <c r="DI1" s="108"/>
-      <c r="DJ1" s="108"/>
-      <c r="DK1" s="108"/>
-      <c r="DL1" s="108">
+      <c r="DF1" s="119"/>
+      <c r="DG1" s="119"/>
+      <c r="DH1" s="119"/>
+      <c r="DI1" s="119"/>
+      <c r="DJ1" s="119"/>
+      <c r="DK1" s="119"/>
+      <c r="DL1" s="119">
         <f t="shared" ref="DL1" si="13">DE1+7</f>
         <v>42233</v>
       </c>
-      <c r="DM1" s="108"/>
-      <c r="DN1" s="108"/>
-      <c r="DO1" s="108"/>
-      <c r="DP1" s="108"/>
-      <c r="DQ1" s="108"/>
-      <c r="DR1" s="108"/>
-      <c r="DS1" s="108">
+      <c r="DM1" s="119"/>
+      <c r="DN1" s="119"/>
+      <c r="DO1" s="119"/>
+      <c r="DP1" s="119"/>
+      <c r="DQ1" s="119"/>
+      <c r="DR1" s="119"/>
+      <c r="DS1" s="119">
         <f t="shared" ref="DS1" si="14">DL1+7</f>
         <v>42240</v>
       </c>
-      <c r="DT1" s="108"/>
-      <c r="DU1" s="108"/>
-      <c r="DV1" s="108"/>
-      <c r="DW1" s="108"/>
-      <c r="DX1" s="108"/>
-      <c r="DY1" s="108"/>
-      <c r="DZ1" s="108">
+      <c r="DT1" s="119"/>
+      <c r="DU1" s="119"/>
+      <c r="DV1" s="119"/>
+      <c r="DW1" s="119"/>
+      <c r="DX1" s="119"/>
+      <c r="DY1" s="119"/>
+      <c r="DZ1" s="119">
         <f t="shared" ref="DZ1" si="15">DS1+7</f>
         <v>42247</v>
       </c>
-      <c r="EA1" s="108"/>
-      <c r="EB1" s="108"/>
-      <c r="EC1" s="108"/>
-      <c r="ED1" s="108"/>
-      <c r="EE1" s="108"/>
-      <c r="EF1" s="108"/>
+      <c r="EA1" s="119"/>
+      <c r="EB1" s="119"/>
+      <c r="EC1" s="119"/>
+      <c r="ED1" s="119"/>
+      <c r="EE1" s="119"/>
+      <c r="EF1" s="119"/>
       <c r="EG1" s="27"/>
     </row>
     <row r="2" spans="1:137" s="9" customFormat="1" ht="34" customHeight="1" thickBot="1">
-      <c r="A2" s="115"/>
-      <c r="B2" s="113"/>
-      <c r="C2" s="115"/>
+      <c r="A2" s="118"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="118"/>
       <c r="D2" s="8" t="s">
         <v>1</v>
       </c>
@@ -3071,10 +3089,10 @@
         <f>SUM(D4:EF4)</f>
         <v>8</v>
       </c>
-      <c r="D4" s="97">
+      <c r="D4" s="96">
         <v>8</v>
       </c>
-      <c r="E4" s="98"/>
+      <c r="E4" s="97"/>
       <c r="F4" s="77"/>
       <c r="J4" s="30"/>
       <c r="K4" s="17"/>
@@ -3127,11 +3145,11 @@
         <v>2</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="99">
+      <c r="E5" s="98">
         <v>2</v>
       </c>
-      <c r="F5" s="98"/>
-      <c r="G5" s="99"/>
+      <c r="F5" s="97"/>
+      <c r="G5" s="98"/>
     </row>
     <row r="6" spans="1:137" s="13" customFormat="1" ht="41" customHeight="1" thickBot="1">
       <c r="A6" s="10" t="s">
@@ -3144,17 +3162,17 @@
         <f>SUM(D6:EF6)</f>
         <v>16</v>
       </c>
-      <c r="D6" s="100"/>
-      <c r="E6" s="100">
+      <c r="D6" s="99"/>
+      <c r="E6" s="99">
         <v>6</v>
       </c>
-      <c r="F6" s="101">
+      <c r="F6" s="100">
         <v>8</v>
       </c>
-      <c r="G6" s="100">
+      <c r="G6" s="99">
         <v>2</v>
       </c>
-      <c r="I6" s="99"/>
+      <c r="I6" s="98"/>
       <c r="J6" s="70"/>
       <c r="K6" s="71"/>
       <c r="Q6" s="32"/>
@@ -3258,12 +3276,12 @@
         <v>4</v>
       </c>
       <c r="D8" s="17"/>
-      <c r="G8" s="97">
+      <c r="G8" s="96">
         <v>4</v>
       </c>
-      <c r="H8" s="97"/>
+      <c r="H8" s="96"/>
       <c r="J8" s="30"/>
-      <c r="K8" s="103"/>
+      <c r="K8" s="102"/>
       <c r="L8" s="22"/>
       <c r="N8" s="37"/>
       <c r="O8" s="37"/>
@@ -3328,13 +3346,13 @@
         <f>SUM(D9:EF9)</f>
         <v>12</v>
       </c>
-      <c r="G9" s="99">
+      <c r="G9" s="98">
         <v>2</v>
       </c>
-      <c r="H9" s="99">
+      <c r="H9" s="98">
         <v>8</v>
       </c>
-      <c r="K9" s="102">
+      <c r="K9" s="101">
         <v>2</v>
       </c>
       <c r="N9" s="64"/>
@@ -3370,25 +3388,25 @@
       </c>
       <c r="D10" s="12"/>
       <c r="J10" s="32"/>
-      <c r="K10" s="101">
+      <c r="K10" s="100">
         <v>6</v>
       </c>
-      <c r="L10" s="100">
+      <c r="L10" s="99">
         <v>6</v>
       </c>
-      <c r="M10" s="105"/>
-      <c r="N10" s="105"/>
+      <c r="M10" s="104"/>
+      <c r="N10" s="104"/>
       <c r="O10" s="65"/>
       <c r="P10" s="34"/>
       <c r="Q10" s="72"/>
-      <c r="R10" s="106"/>
-      <c r="S10" s="105"/>
+      <c r="R10" s="105"/>
+      <c r="S10" s="104"/>
       <c r="T10" s="34"/>
       <c r="U10" s="77"/>
       <c r="X10" s="32"/>
-      <c r="Y10" s="106"/>
-      <c r="Z10" s="105"/>
-      <c r="AA10" s="105"/>
+      <c r="Y10" s="105"/>
+      <c r="Z10" s="104"/>
+      <c r="AA10" s="104"/>
       <c r="AB10" s="34"/>
       <c r="AC10" s="34"/>
       <c r="AD10" s="34"/>
@@ -3498,10 +3516,10 @@
       <c r="I12" s="35"/>
       <c r="J12" s="74"/>
       <c r="K12" s="35"/>
-      <c r="L12" s="97">
+      <c r="L12" s="96">
         <v>2</v>
       </c>
-      <c r="M12" s="97">
+      <c r="M12" s="96">
         <v>2</v>
       </c>
       <c r="N12" s="22"/>
@@ -3560,10 +3578,10 @@
       <c r="J13" s="36"/>
       <c r="K13" s="35"/>
       <c r="L13" s="35"/>
-      <c r="M13" s="99">
+      <c r="M13" s="98">
         <v>6</v>
       </c>
-      <c r="N13" s="25">
+      <c r="N13" s="96">
         <v>2</v>
       </c>
       <c r="O13" s="35"/>
@@ -3573,7 +3591,7 @@
       <c r="S13" s="35"/>
       <c r="T13" s="35"/>
       <c r="U13" s="35"/>
-      <c r="AB13" s="107"/>
+      <c r="AB13" s="106"/>
     </row>
     <row r="14" spans="1:137" ht="41" customHeight="1">
       <c r="A14" s="6" t="s">
@@ -3594,7 +3612,7 @@
       <c r="L14" s="35"/>
       <c r="M14" s="35"/>
       <c r="N14" s="35"/>
-      <c r="O14" s="91">
+      <c r="O14" s="97">
         <v>8</v>
       </c>
       <c r="P14" s="35"/>
@@ -3603,7 +3621,7 @@
       <c r="S14" s="22"/>
       <c r="T14" s="35"/>
       <c r="U14" s="35"/>
-      <c r="AB14" s="107"/>
+      <c r="AB14" s="106"/>
     </row>
     <row r="15" spans="1:137" ht="41" customHeight="1">
       <c r="A15" s="6" t="s">
@@ -3627,13 +3645,13 @@
       <c r="O15" s="35"/>
       <c r="P15" s="35"/>
       <c r="Q15" s="36"/>
-      <c r="R15" s="102">
+      <c r="R15" s="101">
         <v>6</v>
       </c>
       <c r="S15" s="37"/>
       <c r="T15" s="64"/>
       <c r="U15" s="35"/>
-      <c r="AB15" s="107"/>
+      <c r="AB15" s="106"/>
     </row>
     <row r="16" spans="1:137" s="13" customFormat="1" ht="41" customHeight="1" thickBot="1">
       <c r="A16" s="10" t="s">
@@ -3659,14 +3677,14 @@
       <c r="P16" s="34"/>
       <c r="Q16" s="72"/>
       <c r="R16" s="73"/>
-      <c r="S16" s="100">
+      <c r="S16" s="99">
         <v>4</v>
       </c>
       <c r="T16" s="37"/>
       <c r="U16" s="65"/>
       <c r="X16" s="32"/>
       <c r="Y16" s="12"/>
-      <c r="AC16" s="105"/>
+      <c r="AC16" s="104"/>
       <c r="AE16" s="32"/>
       <c r="AF16" s="12"/>
       <c r="AL16" s="32"/>
@@ -3772,14 +3790,14 @@
       <c r="J18" s="36"/>
       <c r="K18" s="4"/>
       <c r="L18" s="35"/>
-      <c r="T18" s="109" t="s">
+      <c r="T18" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="U18" s="110"/>
-      <c r="V18" s="110"/>
-      <c r="W18" s="110"/>
-      <c r="X18" s="111"/>
-      <c r="Y18" s="33">
+      <c r="U18" s="113"/>
+      <c r="V18" s="113"/>
+      <c r="W18" s="113"/>
+      <c r="X18" s="114"/>
+      <c r="Y18" s="101">
         <v>4</v>
       </c>
       <c r="Z18" s="76"/>
@@ -3806,15 +3824,15 @@
       <c r="L19" s="34"/>
       <c r="Q19" s="32"/>
       <c r="R19" s="12"/>
-      <c r="T19" s="109" t="s">
+      <c r="T19" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="U19" s="110"/>
-      <c r="V19" s="110"/>
-      <c r="W19" s="110"/>
-      <c r="X19" s="111"/>
+      <c r="U19" s="113"/>
+      <c r="V19" s="113"/>
+      <c r="W19" s="113"/>
+      <c r="X19" s="114"/>
       <c r="Y19" s="12"/>
-      <c r="Z19" s="24">
+      <c r="Z19" s="99">
         <v>8</v>
       </c>
       <c r="AA19" s="24">
@@ -3930,10 +3948,10 @@
       <c r="X21" s="74"/>
       <c r="Y21" s="75"/>
       <c r="Z21" s="37"/>
-      <c r="AA21" s="103">
+      <c r="AA21" s="102">
         <v>2</v>
       </c>
-      <c r="AB21" s="92"/>
+      <c r="AB21" s="91"/>
       <c r="AE21" s="74"/>
       <c r="AF21" s="75"/>
       <c r="AG21" s="77"/>
@@ -3990,15 +4008,15 @@
       <c r="X22" s="36"/>
       <c r="Y22" s="4"/>
       <c r="Z22" s="35"/>
-      <c r="AA22" s="33">
+      <c r="AA22" s="101">
         <v>1</v>
       </c>
-      <c r="AB22" s="93"/>
+      <c r="AB22" s="92"/>
       <c r="AE22" s="36"/>
       <c r="AF22" s="4"/>
       <c r="AG22" s="77"/>
       <c r="AH22" s="35"/>
-      <c r="AI22" s="35"/>
+      <c r="AI22" s="106"/>
       <c r="AJ22" s="35"/>
     </row>
     <row r="23" spans="1:137" ht="41" customHeight="1">
@@ -4020,17 +4038,17 @@
       <c r="X23" s="36"/>
       <c r="Y23" s="4"/>
       <c r="Z23" s="37"/>
-      <c r="AA23" s="33">
+      <c r="AA23" s="101">
         <v>1</v>
       </c>
-      <c r="AB23" s="23">
+      <c r="AB23" s="98">
         <v>5</v>
       </c>
       <c r="AE23" s="36"/>
-      <c r="AF23" s="94"/>
+      <c r="AF23" s="93"/>
       <c r="AG23" s="35"/>
       <c r="AH23" s="77"/>
-      <c r="AI23" s="35"/>
+      <c r="AI23" s="106"/>
       <c r="AJ23" s="35"/>
     </row>
     <row r="24" spans="1:137" ht="41" customHeight="1">
@@ -4053,7 +4071,7 @@
       <c r="Y24" s="4"/>
       <c r="Z24" s="37"/>
       <c r="AA24" s="4"/>
-      <c r="AB24" s="23">
+      <c r="AB24" s="98">
         <v>2</v>
       </c>
       <c r="AC24" s="64"/>
@@ -4061,7 +4079,7 @@
       <c r="AF24" s="4"/>
       <c r="AG24" s="35"/>
       <c r="AH24" s="77"/>
-      <c r="AI24" s="35"/>
+      <c r="AI24" s="106"/>
       <c r="AJ24" s="35"/>
     </row>
     <row r="25" spans="1:137" s="13" customFormat="1" ht="41" customHeight="1" thickBot="1">
@@ -4089,17 +4107,17 @@
       <c r="Y25" s="73"/>
       <c r="Z25" s="34"/>
       <c r="AA25" s="73"/>
-      <c r="AB25" s="24">
+      <c r="AB25" s="99">
         <v>1</v>
       </c>
-      <c r="AC25" s="24">
+      <c r="AC25" s="99">
         <v>1</v>
       </c>
       <c r="AE25" s="72"/>
-      <c r="AF25" s="95"/>
+      <c r="AF25" s="94"/>
       <c r="AG25" s="34"/>
       <c r="AH25" s="77"/>
-      <c r="AI25" s="34"/>
+      <c r="AI25" s="104"/>
       <c r="AJ25" s="34"/>
       <c r="AL25" s="32"/>
       <c r="AM25" s="12"/>
@@ -4202,12 +4220,12 @@
       <c r="R27" s="17"/>
       <c r="X27" s="30"/>
       <c r="Y27" s="17"/>
-      <c r="AC27" s="25">
+      <c r="AC27" s="96">
         <v>2</v>
       </c>
       <c r="AD27" s="37"/>
       <c r="AE27" s="74"/>
-      <c r="AF27" s="96"/>
+      <c r="AF27" s="95"/>
       <c r="AG27" s="37"/>
       <c r="AH27" s="77"/>
       <c r="AI27" s="37"/>
@@ -4215,6 +4233,7 @@
       <c r="AK27" s="37"/>
       <c r="AL27" s="30"/>
       <c r="AM27" s="17"/>
+      <c r="AN27" s="107"/>
       <c r="AS27" s="30"/>
       <c r="AT27" s="17"/>
       <c r="AZ27" s="30"/>
@@ -4255,17 +4274,18 @@
         <f t="shared" si="23"/>
         <v>4</v>
       </c>
-      <c r="AC28" s="23">
+      <c r="AC28" s="98">
         <v>4</v>
       </c>
       <c r="AD28" s="35"/>
       <c r="AE28" s="36"/>
-      <c r="AF28" s="94"/>
+      <c r="AF28" s="93"/>
       <c r="AG28" s="37"/>
       <c r="AH28" s="35"/>
       <c r="AI28" s="77"/>
       <c r="AJ28" s="35"/>
       <c r="AK28" s="35"/>
+      <c r="AN28" s="108"/>
     </row>
     <row r="29" spans="1:137" s="13" customFormat="1" ht="41" customHeight="1" thickBot="1">
       <c r="A29" s="10" t="s">
@@ -4288,7 +4308,7 @@
       <c r="AC29" s="34"/>
       <c r="AD29" s="34"/>
       <c r="AE29" s="72"/>
-      <c r="AF29" s="26">
+      <c r="AF29" s="100">
         <v>4</v>
       </c>
       <c r="AG29" s="37"/>
@@ -4298,6 +4318,7 @@
       <c r="AK29" s="34"/>
       <c r="AL29" s="32"/>
       <c r="AM29" s="12"/>
+      <c r="AN29" s="109"/>
       <c r="AS29" s="32"/>
       <c r="AT29" s="12"/>
       <c r="AZ29" s="32"/>
@@ -4398,7 +4419,7 @@
       <c r="X31" s="30"/>
       <c r="Y31" s="17"/>
       <c r="AE31" s="30"/>
-      <c r="AF31" s="38">
+      <c r="AF31" s="102">
         <v>2</v>
       </c>
       <c r="AG31" s="22"/>
@@ -4408,7 +4429,7 @@
       <c r="AK31" s="37"/>
       <c r="AL31" s="74"/>
       <c r="AM31" s="75"/>
-      <c r="AN31" s="37"/>
+      <c r="AN31" s="107"/>
       <c r="AS31" s="30"/>
       <c r="AT31" s="17"/>
       <c r="AZ31" s="30"/>
@@ -4449,10 +4470,10 @@
         <f t="shared" si="23"/>
         <v>4</v>
       </c>
-      <c r="AF32" s="33">
+      <c r="AF32" s="101">
         <v>2</v>
       </c>
-      <c r="AG32" s="23">
+      <c r="AG32" s="98">
         <v>2</v>
       </c>
       <c r="AH32" s="22"/>
@@ -4461,7 +4482,7 @@
       <c r="AK32" s="35"/>
       <c r="AL32" s="36"/>
       <c r="AM32" s="4"/>
-      <c r="AN32" s="35"/>
+      <c r="AN32" s="108"/>
     </row>
     <row r="33" spans="1:137" s="13" customFormat="1" ht="41" customHeight="1" thickBot="1">
       <c r="A33" s="10" t="s">
@@ -4483,7 +4504,7 @@
       <c r="Y33" s="12"/>
       <c r="AE33" s="32"/>
       <c r="AF33" s="12"/>
-      <c r="AG33" s="24">
+      <c r="AG33" s="99">
         <v>4</v>
       </c>
       <c r="AH33" s="34"/>
@@ -4492,7 +4513,7 @@
       <c r="AK33" s="34"/>
       <c r="AL33" s="72"/>
       <c r="AM33" s="77"/>
-      <c r="AN33" s="34"/>
+      <c r="AN33" s="109"/>
       <c r="AS33" s="32"/>
       <c r="AT33" s="12"/>
       <c r="AZ33" s="32"/>
@@ -4594,10 +4615,10 @@
       <c r="Y35" s="17"/>
       <c r="AE35" s="30"/>
       <c r="AF35" s="17"/>
-      <c r="AG35" s="25">
+      <c r="AG35" s="96">
         <v>2</v>
       </c>
-      <c r="AH35" s="25">
+      <c r="AH35" s="96">
         <v>2</v>
       </c>
       <c r="AI35" s="22"/>
@@ -4605,7 +4626,7 @@
       <c r="AK35" s="37"/>
       <c r="AL35" s="74"/>
       <c r="AM35" s="77"/>
-      <c r="AN35" s="37"/>
+      <c r="AN35" s="107"/>
       <c r="AO35" s="37"/>
       <c r="AP35" s="37"/>
       <c r="AS35" s="30"/>
@@ -4648,7 +4669,7 @@
         <f t="shared" si="23"/>
         <v>4</v>
       </c>
-      <c r="AH36" s="23">
+      <c r="AH36" s="98">
         <v>4</v>
       </c>
       <c r="AI36" s="64"/>
@@ -4656,7 +4677,7 @@
       <c r="AK36" s="35"/>
       <c r="AL36" s="36"/>
       <c r="AM36" s="77"/>
-      <c r="AN36" s="35"/>
+      <c r="AN36" s="108"/>
       <c r="AO36" s="35"/>
       <c r="AP36" s="35"/>
     </row>
@@ -4680,17 +4701,17 @@
       <c r="Y37" s="12"/>
       <c r="AE37" s="32"/>
       <c r="AF37" s="12"/>
-      <c r="AH37" s="24">
+      <c r="AH37" s="99">
         <v>2</v>
       </c>
-      <c r="AI37" s="24">
+      <c r="AI37" s="99">
         <v>2</v>
       </c>
       <c r="AJ37" s="37"/>
       <c r="AK37" s="34"/>
       <c r="AL37" s="72"/>
-      <c r="AM37" s="95"/>
-      <c r="AN37" s="34"/>
+      <c r="AM37" s="94"/>
+      <c r="AN37" s="109"/>
       <c r="AO37" s="77"/>
       <c r="AP37" s="34"/>
       <c r="AS37" s="32"/>
@@ -4857,13 +4878,13 @@
       <c r="AE40" s="32"/>
       <c r="AF40" s="12"/>
       <c r="AI40" s="34"/>
-      <c r="AJ40" s="24">
+      <c r="AJ40" s="99">
         <v>4</v>
       </c>
       <c r="AK40" s="34"/>
       <c r="AL40" s="72"/>
-      <c r="AM40" s="95"/>
-      <c r="AN40" s="37"/>
+      <c r="AM40" s="94"/>
+      <c r="AN40" s="111"/>
       <c r="AO40" s="77"/>
       <c r="AP40" s="34"/>
       <c r="AQ40" s="34"/>
@@ -4972,7 +4993,7 @@
       <c r="AD42" s="77"/>
       <c r="AE42" s="30"/>
       <c r="AF42" s="17"/>
-      <c r="AJ42" s="25">
+      <c r="AJ42" s="96">
         <v>2</v>
       </c>
       <c r="AL42" s="30"/>
@@ -5623,44 +5644,44 @@
       <c r="C50" s="15">
         <v>8</v>
       </c>
-      <c r="D50" s="39"/>
-      <c r="E50" s="40"/>
-      <c r="F50" s="40"/>
-      <c r="G50" s="40"/>
-      <c r="H50" s="40"/>
-      <c r="I50" s="40"/>
-      <c r="J50" s="41"/>
-      <c r="K50" s="39"/>
-      <c r="L50" s="40"/>
-      <c r="M50" s="40"/>
-      <c r="N50" s="40"/>
-      <c r="O50" s="40"/>
-      <c r="P50" s="40"/>
-      <c r="Q50" s="41"/>
-      <c r="R50" s="39"/>
-      <c r="S50" s="40"/>
-      <c r="T50" s="40"/>
-      <c r="U50" s="40"/>
-      <c r="V50" s="40"/>
-      <c r="W50" s="40"/>
-      <c r="X50" s="41"/>
-      <c r="Y50" s="39"/>
-      <c r="Z50" s="40"/>
-      <c r="AA50" s="40"/>
-      <c r="AB50" s="40"/>
-      <c r="AC50" s="40"/>
-      <c r="AD50" s="40"/>
-      <c r="AE50" s="41"/>
-      <c r="AF50" s="39"/>
-      <c r="AG50" s="40"/>
-      <c r="AH50" s="40"/>
-      <c r="AI50" s="40"/>
-      <c r="AJ50" s="40"/>
-      <c r="AK50" s="40"/>
-      <c r="AL50" s="41"/>
-      <c r="AM50" s="39"/>
-      <c r="AN50" s="40"/>
-      <c r="AO50" s="40"/>
+      <c r="D50" s="102"/>
+      <c r="E50" s="96"/>
+      <c r="F50" s="96"/>
+      <c r="G50" s="96"/>
+      <c r="H50" s="96"/>
+      <c r="I50" s="96"/>
+      <c r="J50" s="110"/>
+      <c r="K50" s="102"/>
+      <c r="L50" s="96"/>
+      <c r="M50" s="96"/>
+      <c r="N50" s="96"/>
+      <c r="O50" s="96"/>
+      <c r="P50" s="96"/>
+      <c r="Q50" s="110"/>
+      <c r="R50" s="102"/>
+      <c r="S50" s="96"/>
+      <c r="T50" s="96"/>
+      <c r="U50" s="96"/>
+      <c r="V50" s="96"/>
+      <c r="W50" s="96"/>
+      <c r="X50" s="110"/>
+      <c r="Y50" s="102"/>
+      <c r="Z50" s="96"/>
+      <c r="AA50" s="96"/>
+      <c r="AB50" s="96"/>
+      <c r="AC50" s="96"/>
+      <c r="AD50" s="96"/>
+      <c r="AE50" s="110"/>
+      <c r="AF50" s="102"/>
+      <c r="AG50" s="96"/>
+      <c r="AH50" s="96"/>
+      <c r="AI50" s="96"/>
+      <c r="AJ50" s="96"/>
+      <c r="AK50" s="96"/>
+      <c r="AL50" s="110"/>
+      <c r="AM50" s="102"/>
+      <c r="AN50" s="96"/>
+      <c r="AO50" s="96"/>
       <c r="AP50" s="40"/>
       <c r="AQ50" s="25"/>
       <c r="AR50" s="25"/>
@@ -6385,21 +6406,19 @@
       <c r="B66" s="83"/>
     </row>
     <row r="67" spans="1:2" ht="41" customHeight="1" thickBot="1">
-      <c r="A67" s="104" t="s">
+      <c r="A67" s="103" t="s">
         <v>74</v>
       </c>
       <c r="B67" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="T19:X19"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:J1"/>
-    <mergeCell ref="K1:Q1"/>
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="T18:X18"/>
+    <mergeCell ref="DE1:DK1"/>
+    <mergeCell ref="DL1:DR1"/>
+    <mergeCell ref="DS1:DY1"/>
+    <mergeCell ref="DZ1:EF1"/>
+    <mergeCell ref="CQ1:CW1"/>
+    <mergeCell ref="CX1:DD1"/>
     <mergeCell ref="BO1:BU1"/>
     <mergeCell ref="BV1:CB1"/>
     <mergeCell ref="CC1:CI1"/>
@@ -6410,12 +6429,14 @@
     <mergeCell ref="AT1:AZ1"/>
     <mergeCell ref="BA1:BG1"/>
     <mergeCell ref="BH1:BN1"/>
-    <mergeCell ref="DE1:DK1"/>
-    <mergeCell ref="DL1:DR1"/>
-    <mergeCell ref="DS1:DY1"/>
-    <mergeCell ref="DZ1:EF1"/>
-    <mergeCell ref="CQ1:CW1"/>
-    <mergeCell ref="CX1:DD1"/>
+    <mergeCell ref="T19:X19"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="K1:Q1"/>
+    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="T18:X18"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>